<commit_message>
nmv 29 03 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 7.1 TO 7.5.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 7.1 TO 7.5.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A642B7-EF72-4675-84B7-39A63164154E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772E04F1-B983-44F5-AFD8-1D36EB35CBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="7.1" sheetId="15" r:id="rId1"/>
-    <sheet name="total 7.1 to 7.5" sheetId="7" r:id="rId2"/>
+    <sheet name="7.2" sheetId="16" r:id="rId2"/>
+    <sheet name="total 7.1 to 7.5" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="156">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1546,6 +1547,159 @@
   </si>
   <si>
     <t>52</t>
+  </si>
+  <si>
+    <t>7.2.1.1 :</t>
+  </si>
+  <si>
+    <t>7.2.1.2 :</t>
+  </si>
+  <si>
+    <t>7.2.1.3 :</t>
+  </si>
+  <si>
+    <t>7.2.1.4 :</t>
+  </si>
+  <si>
+    <t>7.2.2.1 :</t>
+  </si>
+  <si>
+    <t>7.2.2.2 :</t>
+  </si>
+  <si>
+    <t>7.2.2.3 :</t>
+  </si>
+  <si>
+    <t>7.2.3.1 :</t>
+  </si>
+  <si>
+    <t>7.2.3.2 :</t>
+  </si>
+  <si>
+    <t>7.2.4.1 :</t>
+  </si>
+  <si>
+    <t>7.2.4.2 :</t>
+  </si>
+  <si>
+    <t>7.2.4.3 :</t>
+  </si>
+  <si>
+    <t>7.2.5.1 :</t>
+  </si>
+  <si>
+    <t>7.2.5.2 :</t>
+  </si>
+  <si>
+    <t>7.2.5.3 :</t>
+  </si>
+  <si>
+    <t>7.2.5.4 :</t>
+  </si>
+  <si>
+    <t>7.2.5.5 :</t>
+  </si>
+  <si>
+    <t>7.2.5.6 :</t>
+  </si>
+  <si>
+    <t>7.2.6.1 :</t>
+  </si>
+  <si>
+    <t>7.2.6.2 :</t>
+  </si>
+  <si>
+    <t>7.2.6.3 :</t>
+  </si>
+  <si>
+    <t>7.2.7.1 :</t>
+  </si>
+  <si>
+    <t>7.2.7.2 :</t>
+  </si>
+  <si>
+    <t>7.2.7.3 :</t>
+  </si>
+  <si>
+    <t>7.2.7.4 :</t>
+  </si>
+  <si>
+    <t>7.2.7.5 :</t>
+  </si>
+  <si>
+    <t>7.2.8.1 :</t>
+  </si>
+  <si>
+    <t>7.2.8.2 :</t>
+  </si>
+  <si>
+    <t>7.2.8.3 :</t>
+  </si>
+  <si>
+    <t>7.2.8.4 :</t>
+  </si>
+  <si>
+    <t>7.2.8.5 :</t>
+  </si>
+  <si>
+    <t>7.2.8.6 :</t>
+  </si>
+  <si>
+    <t>7.2.8.7 :</t>
+  </si>
+  <si>
+    <t>7.2.9.1 :</t>
+  </si>
+  <si>
+    <t>7.2.9.2 :</t>
+  </si>
+  <si>
+    <t>7.2.9.3 :</t>
+  </si>
+  <si>
+    <t>7.2.10.1 :</t>
+  </si>
+  <si>
+    <t>7.2.10.2 :</t>
+  </si>
+  <si>
+    <t>7.2.10.3 :</t>
+  </si>
+  <si>
+    <t>7.2.10.4 :</t>
+  </si>
+  <si>
+    <t>7.2.11.1 :</t>
+  </si>
+  <si>
+    <t>7.2.12.1 :</t>
+  </si>
+  <si>
+    <t>7.2.13.1 :</t>
+  </si>
+  <si>
+    <t>7.2.14.1 :</t>
+  </si>
+  <si>
+    <t>7.2.15.1 :</t>
+  </si>
+  <si>
+    <t>7.2.16.1 :</t>
+  </si>
+  <si>
+    <t>7.2.17.1 :</t>
+  </si>
+  <si>
+    <t>7.2.18.1 :</t>
+  </si>
+  <si>
+    <t>7.2.19.1 :</t>
+  </si>
+  <si>
+    <t>7.2.20.1 :</t>
+  </si>
+  <si>
+    <t>50</t>
   </si>
 </sst>
 </file>
@@ -2132,8 +2286,2191 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L63"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55:J63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="32">
+        <v>10</v>
+      </c>
+      <c r="C2" s="32">
+        <v>0</v>
+      </c>
+      <c r="D2" s="32">
+        <v>0</v>
+      </c>
+      <c r="E2" s="32">
+        <v>0</v>
+      </c>
+      <c r="F2" s="32">
+        <v>0</v>
+      </c>
+      <c r="G2" s="32">
+        <v>3</v>
+      </c>
+      <c r="H2" s="32">
+        <v>0</v>
+      </c>
+      <c r="I2" s="32">
+        <v>0</v>
+      </c>
+      <c r="J2" s="32">
+        <v>40</v>
+      </c>
+      <c r="K2" s="32">
+        <v>50</v>
+      </c>
+      <c r="L2" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="32">
+        <v>9</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0</v>
+      </c>
+      <c r="D3" s="32">
+        <v>2</v>
+      </c>
+      <c r="E3" s="32">
+        <v>0</v>
+      </c>
+      <c r="F3" s="32">
+        <v>0</v>
+      </c>
+      <c r="G3" s="32">
+        <v>6</v>
+      </c>
+      <c r="H3" s="32">
+        <v>0</v>
+      </c>
+      <c r="I3" s="32">
+        <v>0</v>
+      </c>
+      <c r="J3" s="32">
+        <v>39</v>
+      </c>
+      <c r="K3" s="32">
+        <v>50</v>
+      </c>
+      <c r="L3" s="32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="32">
+        <v>10</v>
+      </c>
+      <c r="C4" s="32">
+        <v>0</v>
+      </c>
+      <c r="D4" s="32">
+        <v>2</v>
+      </c>
+      <c r="E4" s="32">
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <v>0</v>
+      </c>
+      <c r="G4" s="32">
+        <v>6</v>
+      </c>
+      <c r="H4" s="32">
+        <v>0</v>
+      </c>
+      <c r="I4" s="32">
+        <v>0</v>
+      </c>
+      <c r="J4" s="32">
+        <v>38</v>
+      </c>
+      <c r="K4" s="32">
+        <v>50</v>
+      </c>
+      <c r="L4" s="32">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="32">
+        <v>6</v>
+      </c>
+      <c r="C5" s="32">
+        <v>0</v>
+      </c>
+      <c r="D5" s="32">
+        <v>0</v>
+      </c>
+      <c r="E5" s="32">
+        <v>0</v>
+      </c>
+      <c r="F5" s="32">
+        <v>0</v>
+      </c>
+      <c r="G5" s="32">
+        <v>5</v>
+      </c>
+      <c r="H5" s="32">
+        <v>0</v>
+      </c>
+      <c r="I5" s="32">
+        <v>0</v>
+      </c>
+      <c r="J5" s="32">
+        <v>44</v>
+      </c>
+      <c r="K5" s="32">
+        <v>50</v>
+      </c>
+      <c r="L5" s="32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="32">
+        <v>5</v>
+      </c>
+      <c r="C6" s="32">
+        <v>0</v>
+      </c>
+      <c r="D6" s="32">
+        <v>0</v>
+      </c>
+      <c r="E6" s="32">
+        <v>0</v>
+      </c>
+      <c r="F6" s="32">
+        <v>0</v>
+      </c>
+      <c r="G6" s="32">
+        <v>4</v>
+      </c>
+      <c r="H6" s="32">
+        <v>0</v>
+      </c>
+      <c r="I6" s="32">
+        <v>0</v>
+      </c>
+      <c r="J6" s="32">
+        <v>45</v>
+      </c>
+      <c r="K6" s="32">
+        <v>50</v>
+      </c>
+      <c r="L6" s="32">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="32">
+        <v>10</v>
+      </c>
+      <c r="C7" s="32">
+        <v>0</v>
+      </c>
+      <c r="D7" s="32">
+        <v>0</v>
+      </c>
+      <c r="E7" s="32">
+        <v>0</v>
+      </c>
+      <c r="F7" s="32">
+        <v>1</v>
+      </c>
+      <c r="G7" s="32">
+        <v>4</v>
+      </c>
+      <c r="H7" s="32">
+        <v>0</v>
+      </c>
+      <c r="I7" s="32">
+        <v>0</v>
+      </c>
+      <c r="J7" s="32">
+        <v>48</v>
+      </c>
+      <c r="K7" s="32">
+        <v>59</v>
+      </c>
+      <c r="L7" s="32">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="32">
+        <v>11</v>
+      </c>
+      <c r="C8" s="32">
+        <v>0</v>
+      </c>
+      <c r="D8" s="32">
+        <v>1</v>
+      </c>
+      <c r="E8" s="32">
+        <v>0</v>
+      </c>
+      <c r="F8" s="32">
+        <v>1</v>
+      </c>
+      <c r="G8" s="32">
+        <v>3</v>
+      </c>
+      <c r="H8" s="32">
+        <v>0</v>
+      </c>
+      <c r="I8" s="32">
+        <v>0</v>
+      </c>
+      <c r="J8" s="32">
+        <v>50</v>
+      </c>
+      <c r="K8" s="32">
+        <v>63</v>
+      </c>
+      <c r="L8" s="32">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="32">
+        <v>11</v>
+      </c>
+      <c r="C9" s="32">
+        <v>0</v>
+      </c>
+      <c r="D9" s="32">
+        <v>0</v>
+      </c>
+      <c r="E9" s="32">
+        <v>0</v>
+      </c>
+      <c r="F9" s="32">
+        <v>0</v>
+      </c>
+      <c r="G9" s="32">
+        <v>2</v>
+      </c>
+      <c r="H9" s="32">
+        <v>0</v>
+      </c>
+      <c r="I9" s="32">
+        <v>0</v>
+      </c>
+      <c r="J9" s="32">
+        <v>39</v>
+      </c>
+      <c r="K9" s="32">
+        <v>50</v>
+      </c>
+      <c r="L9" s="32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="32">
+        <v>10</v>
+      </c>
+      <c r="C10" s="32">
+        <v>0</v>
+      </c>
+      <c r="D10" s="32">
+        <v>0</v>
+      </c>
+      <c r="E10" s="32">
+        <v>0</v>
+      </c>
+      <c r="F10" s="32">
+        <v>0</v>
+      </c>
+      <c r="G10" s="32">
+        <v>3</v>
+      </c>
+      <c r="H10" s="32">
+        <v>0</v>
+      </c>
+      <c r="I10" s="32">
+        <v>0</v>
+      </c>
+      <c r="J10" s="32">
+        <v>40</v>
+      </c>
+      <c r="K10" s="32">
+        <v>50</v>
+      </c>
+      <c r="L10" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="32">
+        <v>4</v>
+      </c>
+      <c r="C11" s="32">
+        <v>0</v>
+      </c>
+      <c r="D11" s="32">
+        <v>0</v>
+      </c>
+      <c r="E11" s="32">
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <v>1</v>
+      </c>
+      <c r="G11" s="32">
+        <v>1</v>
+      </c>
+      <c r="H11" s="32">
+        <v>0</v>
+      </c>
+      <c r="I11" s="32">
+        <v>0</v>
+      </c>
+      <c r="J11" s="32">
+        <v>39</v>
+      </c>
+      <c r="K11" s="32">
+        <v>44</v>
+      </c>
+      <c r="L11" s="32">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="32">
+        <v>8</v>
+      </c>
+      <c r="C12" s="32">
+        <v>0</v>
+      </c>
+      <c r="D12" s="32">
+        <v>0</v>
+      </c>
+      <c r="E12" s="32">
+        <v>0</v>
+      </c>
+      <c r="F12" s="32">
+        <v>0</v>
+      </c>
+      <c r="G12" s="32">
+        <v>1</v>
+      </c>
+      <c r="H12" s="32">
+        <v>0</v>
+      </c>
+      <c r="I12" s="32">
+        <v>0</v>
+      </c>
+      <c r="J12" s="32">
+        <v>42</v>
+      </c>
+      <c r="K12" s="32">
+        <v>50</v>
+      </c>
+      <c r="L12" s="32">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="32">
+        <v>12</v>
+      </c>
+      <c r="C13" s="32">
+        <v>0</v>
+      </c>
+      <c r="D13" s="32">
+        <v>0</v>
+      </c>
+      <c r="E13" s="32">
+        <v>0</v>
+      </c>
+      <c r="F13" s="32">
+        <v>0</v>
+      </c>
+      <c r="G13" s="32">
+        <v>1</v>
+      </c>
+      <c r="H13" s="32">
+        <v>0</v>
+      </c>
+      <c r="I13" s="32">
+        <v>0</v>
+      </c>
+      <c r="J13" s="32">
+        <v>38</v>
+      </c>
+      <c r="K13" s="32">
+        <v>50</v>
+      </c>
+      <c r="L13" s="32">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="32">
+        <v>14</v>
+      </c>
+      <c r="C14" s="32">
+        <v>1</v>
+      </c>
+      <c r="D14" s="32">
+        <v>1</v>
+      </c>
+      <c r="E14" s="32">
+        <v>0</v>
+      </c>
+      <c r="F14" s="32">
+        <v>1</v>
+      </c>
+      <c r="G14" s="32">
+        <v>3</v>
+      </c>
+      <c r="H14" s="32">
+        <v>0</v>
+      </c>
+      <c r="I14" s="32">
+        <v>0</v>
+      </c>
+      <c r="J14" s="32">
+        <v>56</v>
+      </c>
+      <c r="K14" s="32">
+        <v>71</v>
+      </c>
+      <c r="L14" s="32">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="32">
+        <v>5</v>
+      </c>
+      <c r="C15" s="32">
+        <v>0</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0</v>
+      </c>
+      <c r="E15" s="32">
+        <v>0</v>
+      </c>
+      <c r="F15" s="32">
+        <v>0</v>
+      </c>
+      <c r="G15" s="32">
+        <v>3</v>
+      </c>
+      <c r="H15" s="32">
+        <v>0</v>
+      </c>
+      <c r="I15" s="32">
+        <v>0</v>
+      </c>
+      <c r="J15" s="32">
+        <v>45</v>
+      </c>
+      <c r="K15" s="32">
+        <v>50</v>
+      </c>
+      <c r="L15" s="32">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="32">
+        <v>7</v>
+      </c>
+      <c r="C16" s="32">
+        <v>0</v>
+      </c>
+      <c r="D16" s="32">
+        <v>0</v>
+      </c>
+      <c r="E16" s="32">
+        <v>0</v>
+      </c>
+      <c r="F16" s="32">
+        <v>0</v>
+      </c>
+      <c r="G16" s="32">
+        <v>3</v>
+      </c>
+      <c r="H16" s="32">
+        <v>0</v>
+      </c>
+      <c r="I16" s="32">
+        <v>0</v>
+      </c>
+      <c r="J16" s="32">
+        <v>43</v>
+      </c>
+      <c r="K16" s="32">
+        <v>50</v>
+      </c>
+      <c r="L16" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="32">
+        <v>5</v>
+      </c>
+      <c r="C17" s="32">
+        <v>0</v>
+      </c>
+      <c r="D17" s="32">
+        <v>0</v>
+      </c>
+      <c r="E17" s="32">
+        <v>0</v>
+      </c>
+      <c r="F17" s="32">
+        <v>0</v>
+      </c>
+      <c r="G17" s="32">
+        <v>0</v>
+      </c>
+      <c r="H17" s="32">
+        <v>0</v>
+      </c>
+      <c r="I17" s="32">
+        <v>0</v>
+      </c>
+      <c r="J17" s="32">
+        <v>45</v>
+      </c>
+      <c r="K17" s="32">
+        <v>50</v>
+      </c>
+      <c r="L17" s="32">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="32">
+        <v>14</v>
+      </c>
+      <c r="C18" s="32">
+        <v>0</v>
+      </c>
+      <c r="D18" s="32">
+        <v>0</v>
+      </c>
+      <c r="E18" s="32">
+        <v>0</v>
+      </c>
+      <c r="F18" s="32">
+        <v>0</v>
+      </c>
+      <c r="G18" s="32">
+        <v>1</v>
+      </c>
+      <c r="H18" s="32">
+        <v>0</v>
+      </c>
+      <c r="I18" s="32">
+        <v>0</v>
+      </c>
+      <c r="J18" s="32">
+        <v>36</v>
+      </c>
+      <c r="K18" s="32">
+        <v>50</v>
+      </c>
+      <c r="L18" s="32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="32">
+        <v>7</v>
+      </c>
+      <c r="C19" s="32">
+        <v>0</v>
+      </c>
+      <c r="D19" s="32">
+        <v>0</v>
+      </c>
+      <c r="E19" s="32">
+        <v>0</v>
+      </c>
+      <c r="F19" s="32">
+        <v>0</v>
+      </c>
+      <c r="G19" s="32">
+        <v>2</v>
+      </c>
+      <c r="H19" s="32">
+        <v>0</v>
+      </c>
+      <c r="I19" s="32">
+        <v>0</v>
+      </c>
+      <c r="J19" s="32">
+        <v>43</v>
+      </c>
+      <c r="K19" s="32">
+        <v>50</v>
+      </c>
+      <c r="L19" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="32">
+        <v>9</v>
+      </c>
+      <c r="C20" s="32">
+        <v>0</v>
+      </c>
+      <c r="D20" s="32">
+        <v>0</v>
+      </c>
+      <c r="E20" s="32">
+        <v>0</v>
+      </c>
+      <c r="F20" s="32">
+        <v>0</v>
+      </c>
+      <c r="G20" s="32">
+        <v>0</v>
+      </c>
+      <c r="H20" s="32">
+        <v>0</v>
+      </c>
+      <c r="I20" s="32">
+        <v>0</v>
+      </c>
+      <c r="J20" s="32">
+        <v>41</v>
+      </c>
+      <c r="K20" s="32">
+        <v>50</v>
+      </c>
+      <c r="L20" s="32">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="32">
+        <v>11</v>
+      </c>
+      <c r="C21" s="32">
+        <v>1</v>
+      </c>
+      <c r="D21" s="32">
+        <v>0</v>
+      </c>
+      <c r="E21" s="32">
+        <v>0</v>
+      </c>
+      <c r="F21" s="32">
+        <v>1</v>
+      </c>
+      <c r="G21" s="32">
+        <v>0</v>
+      </c>
+      <c r="H21" s="32">
+        <v>0</v>
+      </c>
+      <c r="I21" s="32">
+        <v>0</v>
+      </c>
+      <c r="J21" s="32">
+        <v>36</v>
+      </c>
+      <c r="K21" s="32">
+        <v>47</v>
+      </c>
+      <c r="L21" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="32">
+        <v>1</v>
+      </c>
+      <c r="C22" s="32">
+        <v>0</v>
+      </c>
+      <c r="D22" s="32">
+        <v>0</v>
+      </c>
+      <c r="E22" s="32">
+        <v>0</v>
+      </c>
+      <c r="F22" s="32">
+        <v>0</v>
+      </c>
+      <c r="G22" s="32">
+        <v>3</v>
+      </c>
+      <c r="H22" s="32">
+        <v>0</v>
+      </c>
+      <c r="I22" s="32">
+        <v>0</v>
+      </c>
+      <c r="J22" s="32">
+        <v>49</v>
+      </c>
+      <c r="K22" s="32">
+        <v>50</v>
+      </c>
+      <c r="L22" s="32">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="32">
+        <v>10</v>
+      </c>
+      <c r="C23" s="32">
+        <v>0</v>
+      </c>
+      <c r="D23" s="32">
+        <v>0</v>
+      </c>
+      <c r="E23" s="32">
+        <v>0</v>
+      </c>
+      <c r="F23" s="32">
+        <v>0</v>
+      </c>
+      <c r="G23" s="32">
+        <v>4</v>
+      </c>
+      <c r="H23" s="32">
+        <v>0</v>
+      </c>
+      <c r="I23" s="32">
+        <v>0</v>
+      </c>
+      <c r="J23" s="32">
+        <v>40</v>
+      </c>
+      <c r="K23" s="32">
+        <v>50</v>
+      </c>
+      <c r="L23" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="32">
+        <v>10</v>
+      </c>
+      <c r="C24" s="32">
+        <v>0</v>
+      </c>
+      <c r="D24" s="32">
+        <v>0</v>
+      </c>
+      <c r="E24" s="32">
+        <v>0</v>
+      </c>
+      <c r="F24" s="32">
+        <v>0</v>
+      </c>
+      <c r="G24" s="32">
+        <v>1</v>
+      </c>
+      <c r="H24" s="32">
+        <v>0</v>
+      </c>
+      <c r="I24" s="32">
+        <v>0</v>
+      </c>
+      <c r="J24" s="32">
+        <v>40</v>
+      </c>
+      <c r="K24" s="32">
+        <v>50</v>
+      </c>
+      <c r="L24" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="32">
+        <v>12</v>
+      </c>
+      <c r="C25" s="32">
+        <v>0</v>
+      </c>
+      <c r="D25" s="32">
+        <v>0</v>
+      </c>
+      <c r="E25" s="32">
+        <v>0</v>
+      </c>
+      <c r="F25" s="32">
+        <v>0</v>
+      </c>
+      <c r="G25" s="32">
+        <v>1</v>
+      </c>
+      <c r="H25" s="32">
+        <v>0</v>
+      </c>
+      <c r="I25" s="32">
+        <v>0</v>
+      </c>
+      <c r="J25" s="32">
+        <v>38</v>
+      </c>
+      <c r="K25" s="32">
+        <v>50</v>
+      </c>
+      <c r="L25" s="32">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="32">
+        <v>5</v>
+      </c>
+      <c r="C26" s="32">
+        <v>0</v>
+      </c>
+      <c r="D26" s="32">
+        <v>0</v>
+      </c>
+      <c r="E26" s="32">
+        <v>0</v>
+      </c>
+      <c r="F26" s="32">
+        <v>0</v>
+      </c>
+      <c r="G26" s="32">
+        <v>0</v>
+      </c>
+      <c r="H26" s="32">
+        <v>0</v>
+      </c>
+      <c r="I26" s="32">
+        <v>0</v>
+      </c>
+      <c r="J26" s="32">
+        <v>45</v>
+      </c>
+      <c r="K26" s="32">
+        <v>50</v>
+      </c>
+      <c r="L26" s="32">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="32">
+        <v>12</v>
+      </c>
+      <c r="C27" s="32">
+        <v>0</v>
+      </c>
+      <c r="D27" s="32">
+        <v>0</v>
+      </c>
+      <c r="E27" s="32">
+        <v>0</v>
+      </c>
+      <c r="F27" s="32">
+        <v>0</v>
+      </c>
+      <c r="G27" s="32">
+        <v>6</v>
+      </c>
+      <c r="H27" s="32">
+        <v>0</v>
+      </c>
+      <c r="I27" s="32">
+        <v>0</v>
+      </c>
+      <c r="J27" s="32">
+        <v>38</v>
+      </c>
+      <c r="K27" s="32">
+        <v>50</v>
+      </c>
+      <c r="L27" s="32">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="32">
+        <v>7</v>
+      </c>
+      <c r="C28" s="32">
+        <v>0</v>
+      </c>
+      <c r="D28" s="32">
+        <v>2</v>
+      </c>
+      <c r="E28" s="32">
+        <v>0</v>
+      </c>
+      <c r="F28" s="32">
+        <v>1</v>
+      </c>
+      <c r="G28" s="32">
+        <v>3</v>
+      </c>
+      <c r="H28" s="32">
+        <v>0</v>
+      </c>
+      <c r="I28" s="32">
+        <v>0</v>
+      </c>
+      <c r="J28" s="32">
+        <v>40</v>
+      </c>
+      <c r="K28" s="32">
+        <v>50</v>
+      </c>
+      <c r="L28" s="32">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="32">
+        <v>3</v>
+      </c>
+      <c r="C29" s="32">
+        <v>0</v>
+      </c>
+      <c r="D29" s="32">
+        <v>0</v>
+      </c>
+      <c r="E29" s="32">
+        <v>0</v>
+      </c>
+      <c r="F29" s="32">
+        <v>1</v>
+      </c>
+      <c r="G29" s="32">
+        <v>4</v>
+      </c>
+      <c r="H29" s="32">
+        <v>0</v>
+      </c>
+      <c r="I29" s="32">
+        <v>0</v>
+      </c>
+      <c r="J29" s="32">
+        <v>35</v>
+      </c>
+      <c r="K29" s="32">
+        <v>39</v>
+      </c>
+      <c r="L29" s="32">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="32">
+        <v>5</v>
+      </c>
+      <c r="C30" s="32">
+        <v>0</v>
+      </c>
+      <c r="D30" s="32">
+        <v>0</v>
+      </c>
+      <c r="E30" s="32">
+        <v>0</v>
+      </c>
+      <c r="F30" s="32">
+        <v>0</v>
+      </c>
+      <c r="G30" s="32">
+        <v>0</v>
+      </c>
+      <c r="H30" s="32">
+        <v>0</v>
+      </c>
+      <c r="I30" s="32">
+        <v>0</v>
+      </c>
+      <c r="J30" s="32">
+        <v>45</v>
+      </c>
+      <c r="K30" s="32">
+        <v>50</v>
+      </c>
+      <c r="L30" s="32">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="32">
+        <v>11</v>
+      </c>
+      <c r="C31" s="32">
+        <v>0</v>
+      </c>
+      <c r="D31" s="32">
+        <v>0</v>
+      </c>
+      <c r="E31" s="32">
+        <v>0</v>
+      </c>
+      <c r="F31" s="32">
+        <v>0</v>
+      </c>
+      <c r="G31" s="32">
+        <v>2</v>
+      </c>
+      <c r="H31" s="32">
+        <v>0</v>
+      </c>
+      <c r="I31" s="32">
+        <v>0</v>
+      </c>
+      <c r="J31" s="32">
+        <v>39</v>
+      </c>
+      <c r="K31" s="32">
+        <v>50</v>
+      </c>
+      <c r="L31" s="32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="32">
+        <v>5</v>
+      </c>
+      <c r="C32" s="32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="32">
+        <v>0</v>
+      </c>
+      <c r="G32" s="32">
+        <v>7</v>
+      </c>
+      <c r="H32" s="32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="32">
+        <v>0</v>
+      </c>
+      <c r="J32" s="32">
+        <v>45</v>
+      </c>
+      <c r="K32" s="32">
+        <v>50</v>
+      </c>
+      <c r="L32" s="32">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="32">
+        <v>13</v>
+      </c>
+      <c r="C33" s="32">
+        <v>0</v>
+      </c>
+      <c r="D33" s="32">
+        <v>0</v>
+      </c>
+      <c r="E33" s="32">
+        <v>0</v>
+      </c>
+      <c r="F33" s="32">
+        <v>1</v>
+      </c>
+      <c r="G33" s="32">
+        <v>9</v>
+      </c>
+      <c r="H33" s="32">
+        <v>0</v>
+      </c>
+      <c r="I33" s="32">
+        <v>0</v>
+      </c>
+      <c r="J33" s="32">
+        <v>48</v>
+      </c>
+      <c r="K33" s="32">
+        <v>62</v>
+      </c>
+      <c r="L33" s="32">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="32">
+        <v>16</v>
+      </c>
+      <c r="C34" s="32">
+        <v>0</v>
+      </c>
+      <c r="D34" s="32">
+        <v>0</v>
+      </c>
+      <c r="E34" s="32">
+        <v>0</v>
+      </c>
+      <c r="F34" s="32">
+        <v>0</v>
+      </c>
+      <c r="G34" s="32">
+        <v>3</v>
+      </c>
+      <c r="H34" s="32">
+        <v>0</v>
+      </c>
+      <c r="I34" s="32">
+        <v>0</v>
+      </c>
+      <c r="J34" s="32">
+        <v>34</v>
+      </c>
+      <c r="K34" s="32">
+        <v>50</v>
+      </c>
+      <c r="L34" s="32">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="32">
+        <v>11</v>
+      </c>
+      <c r="C35" s="32">
+        <v>0</v>
+      </c>
+      <c r="D35" s="32">
+        <v>0</v>
+      </c>
+      <c r="E35" s="32">
+        <v>0</v>
+      </c>
+      <c r="F35" s="32">
+        <v>1</v>
+      </c>
+      <c r="G35" s="32">
+        <v>4</v>
+      </c>
+      <c r="H35" s="32">
+        <v>0</v>
+      </c>
+      <c r="I35" s="32">
+        <v>0</v>
+      </c>
+      <c r="J35" s="32">
+        <v>56</v>
+      </c>
+      <c r="K35" s="32">
+        <v>68</v>
+      </c>
+      <c r="L35" s="32">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="32">
+        <v>7</v>
+      </c>
+      <c r="C36" s="32">
+        <v>0</v>
+      </c>
+      <c r="D36" s="32">
+        <v>1</v>
+      </c>
+      <c r="E36" s="32">
+        <v>0</v>
+      </c>
+      <c r="F36" s="32">
+        <v>1</v>
+      </c>
+      <c r="G36" s="32">
+        <v>3</v>
+      </c>
+      <c r="H36" s="32">
+        <v>0</v>
+      </c>
+      <c r="I36" s="32">
+        <v>0</v>
+      </c>
+      <c r="J36" s="32">
+        <v>39</v>
+      </c>
+      <c r="K36" s="32">
+        <v>48</v>
+      </c>
+      <c r="L36" s="32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="32">
+        <v>6</v>
+      </c>
+      <c r="C37" s="32">
+        <v>0</v>
+      </c>
+      <c r="D37" s="32">
+        <v>0</v>
+      </c>
+      <c r="E37" s="32">
+        <v>0</v>
+      </c>
+      <c r="F37" s="32">
+        <v>0</v>
+      </c>
+      <c r="G37" s="32">
+        <v>3</v>
+      </c>
+      <c r="H37" s="32">
+        <v>0</v>
+      </c>
+      <c r="I37" s="32">
+        <v>0</v>
+      </c>
+      <c r="J37" s="32">
+        <v>44</v>
+      </c>
+      <c r="K37" s="32">
+        <v>50</v>
+      </c>
+      <c r="L37" s="32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="32">
+        <v>7</v>
+      </c>
+      <c r="C38" s="32">
+        <v>0</v>
+      </c>
+      <c r="D38" s="32">
+        <v>0</v>
+      </c>
+      <c r="E38" s="32">
+        <v>0</v>
+      </c>
+      <c r="F38" s="32">
+        <v>0</v>
+      </c>
+      <c r="G38" s="32">
+        <v>6</v>
+      </c>
+      <c r="H38" s="32">
+        <v>0</v>
+      </c>
+      <c r="I38" s="32">
+        <v>0</v>
+      </c>
+      <c r="J38" s="32">
+        <v>43</v>
+      </c>
+      <c r="K38" s="32">
+        <v>50</v>
+      </c>
+      <c r="L38" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="32">
+        <v>12</v>
+      </c>
+      <c r="C39" s="32">
+        <v>0</v>
+      </c>
+      <c r="D39" s="32">
+        <v>1</v>
+      </c>
+      <c r="E39" s="32">
+        <v>0</v>
+      </c>
+      <c r="F39" s="32">
+        <v>0</v>
+      </c>
+      <c r="G39" s="32">
+        <v>0</v>
+      </c>
+      <c r="H39" s="32">
+        <v>0</v>
+      </c>
+      <c r="I39" s="32">
+        <v>0</v>
+      </c>
+      <c r="J39" s="32">
+        <v>37</v>
+      </c>
+      <c r="K39" s="32">
+        <v>50</v>
+      </c>
+      <c r="L39" s="32">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="32">
+        <v>18</v>
+      </c>
+      <c r="C40" s="32">
+        <v>1</v>
+      </c>
+      <c r="D40" s="32">
+        <v>2</v>
+      </c>
+      <c r="E40" s="32">
+        <v>0</v>
+      </c>
+      <c r="F40" s="32">
+        <v>1</v>
+      </c>
+      <c r="G40" s="32">
+        <v>5</v>
+      </c>
+      <c r="H40" s="32">
+        <v>0</v>
+      </c>
+      <c r="I40" s="32">
+        <v>0</v>
+      </c>
+      <c r="J40" s="32">
+        <v>30</v>
+      </c>
+      <c r="K40" s="32">
+        <v>50</v>
+      </c>
+      <c r="L40" s="32">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="32">
+        <v>8</v>
+      </c>
+      <c r="C41" s="32">
+        <v>1</v>
+      </c>
+      <c r="D41" s="32">
+        <v>0</v>
+      </c>
+      <c r="E41" s="32">
+        <v>0</v>
+      </c>
+      <c r="F41" s="32">
+        <v>3</v>
+      </c>
+      <c r="G41" s="32">
+        <v>2</v>
+      </c>
+      <c r="H41" s="32">
+        <v>0</v>
+      </c>
+      <c r="I41" s="32">
+        <v>0</v>
+      </c>
+      <c r="J41" s="32">
+        <v>65</v>
+      </c>
+      <c r="K41" s="32">
+        <v>75</v>
+      </c>
+      <c r="L41" s="32">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="32">
+        <v>8</v>
+      </c>
+      <c r="C42" s="32">
+        <v>0</v>
+      </c>
+      <c r="D42" s="32">
+        <v>0</v>
+      </c>
+      <c r="E42" s="32">
+        <v>0</v>
+      </c>
+      <c r="F42" s="32">
+        <v>1</v>
+      </c>
+      <c r="G42" s="32">
+        <v>1</v>
+      </c>
+      <c r="H42" s="32">
+        <v>0</v>
+      </c>
+      <c r="I42" s="32">
+        <v>0</v>
+      </c>
+      <c r="J42" s="32">
+        <v>63</v>
+      </c>
+      <c r="K42" s="32">
+        <v>72</v>
+      </c>
+      <c r="L42" s="32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="32">
+        <v>11</v>
+      </c>
+      <c r="C43" s="32">
+        <v>0</v>
+      </c>
+      <c r="D43" s="32">
+        <v>0</v>
+      </c>
+      <c r="E43" s="32">
+        <v>0</v>
+      </c>
+      <c r="F43" s="32">
+        <v>1</v>
+      </c>
+      <c r="G43" s="32">
+        <v>0</v>
+      </c>
+      <c r="H43" s="32">
+        <v>0</v>
+      </c>
+      <c r="I43" s="32">
+        <v>0</v>
+      </c>
+      <c r="J43" s="32">
+        <v>14</v>
+      </c>
+      <c r="K43" s="32">
+        <v>26</v>
+      </c>
+      <c r="L43" s="32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="32">
+        <v>0</v>
+      </c>
+      <c r="C44" s="32">
+        <v>0</v>
+      </c>
+      <c r="D44" s="32">
+        <v>0</v>
+      </c>
+      <c r="E44" s="32">
+        <v>0</v>
+      </c>
+      <c r="F44" s="32">
+        <v>1</v>
+      </c>
+      <c r="G44" s="32">
+        <v>0</v>
+      </c>
+      <c r="H44" s="32">
+        <v>0</v>
+      </c>
+      <c r="I44" s="32">
+        <v>0</v>
+      </c>
+      <c r="J44" s="32">
+        <v>22</v>
+      </c>
+      <c r="K44" s="32">
+        <v>23</v>
+      </c>
+      <c r="L44" s="32">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="32">
+        <v>7</v>
+      </c>
+      <c r="C45" s="32">
+        <v>0</v>
+      </c>
+      <c r="D45" s="32">
+        <v>0</v>
+      </c>
+      <c r="E45" s="32">
+        <v>0</v>
+      </c>
+      <c r="F45" s="32">
+        <v>1</v>
+      </c>
+      <c r="G45" s="32">
+        <v>0</v>
+      </c>
+      <c r="H45" s="32">
+        <v>0</v>
+      </c>
+      <c r="I45" s="32">
+        <v>0</v>
+      </c>
+      <c r="J45" s="32">
+        <v>39</v>
+      </c>
+      <c r="K45" s="32">
+        <v>47</v>
+      </c>
+      <c r="L45" s="32">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="32">
+        <v>0</v>
+      </c>
+      <c r="C46" s="32">
+        <v>0</v>
+      </c>
+      <c r="D46" s="32">
+        <v>0</v>
+      </c>
+      <c r="E46" s="32">
+        <v>0</v>
+      </c>
+      <c r="F46" s="32">
+        <v>1</v>
+      </c>
+      <c r="G46" s="32">
+        <v>0</v>
+      </c>
+      <c r="H46" s="32">
+        <v>0</v>
+      </c>
+      <c r="I46" s="32">
+        <v>0</v>
+      </c>
+      <c r="J46" s="32">
+        <v>22</v>
+      </c>
+      <c r="K46" s="32">
+        <v>23</v>
+      </c>
+      <c r="L46" s="32">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="32">
+        <v>3</v>
+      </c>
+      <c r="C47" s="32">
+        <v>0</v>
+      </c>
+      <c r="D47" s="32">
+        <v>0</v>
+      </c>
+      <c r="E47" s="32">
+        <v>0</v>
+      </c>
+      <c r="F47" s="32">
+        <v>1</v>
+      </c>
+      <c r="G47" s="32">
+        <v>0</v>
+      </c>
+      <c r="H47" s="32">
+        <v>0</v>
+      </c>
+      <c r="I47" s="32">
+        <v>0</v>
+      </c>
+      <c r="J47" s="32">
+        <v>40</v>
+      </c>
+      <c r="K47" s="32">
+        <v>44</v>
+      </c>
+      <c r="L47" s="32">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" s="32">
+        <v>2</v>
+      </c>
+      <c r="C48" s="32">
+        <v>0</v>
+      </c>
+      <c r="D48" s="32">
+        <v>0</v>
+      </c>
+      <c r="E48" s="32">
+        <v>0</v>
+      </c>
+      <c r="F48" s="32">
+        <v>0</v>
+      </c>
+      <c r="G48" s="32">
+        <v>0</v>
+      </c>
+      <c r="H48" s="32">
+        <v>0</v>
+      </c>
+      <c r="I48" s="32">
+        <v>0</v>
+      </c>
+      <c r="J48" s="32">
+        <v>48</v>
+      </c>
+      <c r="K48" s="32">
+        <v>50</v>
+      </c>
+      <c r="L48" s="32">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="32">
+        <v>4</v>
+      </c>
+      <c r="C49" s="32">
+        <v>0</v>
+      </c>
+      <c r="D49" s="32">
+        <v>0</v>
+      </c>
+      <c r="E49" s="32">
+        <v>0</v>
+      </c>
+      <c r="F49" s="32">
+        <v>2</v>
+      </c>
+      <c r="G49" s="32">
+        <v>2</v>
+      </c>
+      <c r="H49" s="32">
+        <v>0</v>
+      </c>
+      <c r="I49" s="32">
+        <v>1</v>
+      </c>
+      <c r="J49" s="32">
+        <v>43</v>
+      </c>
+      <c r="K49" s="32">
+        <v>49</v>
+      </c>
+      <c r="L49" s="32">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="32">
+        <v>19</v>
+      </c>
+      <c r="C50" s="32">
+        <v>0</v>
+      </c>
+      <c r="D50" s="32">
+        <v>0</v>
+      </c>
+      <c r="E50" s="32">
+        <v>0</v>
+      </c>
+      <c r="F50" s="32">
+        <v>0</v>
+      </c>
+      <c r="G50" s="32">
+        <v>0</v>
+      </c>
+      <c r="H50" s="32">
+        <v>0</v>
+      </c>
+      <c r="I50" s="32">
+        <v>0</v>
+      </c>
+      <c r="J50" s="32">
+        <v>31</v>
+      </c>
+      <c r="K50" s="32">
+        <v>50</v>
+      </c>
+      <c r="L50" s="32">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="32">
+        <v>10</v>
+      </c>
+      <c r="C51" s="32">
+        <v>0</v>
+      </c>
+      <c r="D51" s="32">
+        <v>0</v>
+      </c>
+      <c r="E51" s="32">
+        <v>0</v>
+      </c>
+      <c r="F51" s="32">
+        <v>0</v>
+      </c>
+      <c r="G51" s="32">
+        <v>0</v>
+      </c>
+      <c r="H51" s="32">
+        <v>0</v>
+      </c>
+      <c r="I51" s="32">
+        <v>0</v>
+      </c>
+      <c r="J51" s="32">
+        <v>40</v>
+      </c>
+      <c r="K51" s="32">
+        <v>50</v>
+      </c>
+      <c r="L51" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="32">
+        <v>22</v>
+      </c>
+      <c r="C52" s="32">
+        <v>0</v>
+      </c>
+      <c r="D52" s="32">
+        <v>0</v>
+      </c>
+      <c r="E52" s="32">
+        <v>0</v>
+      </c>
+      <c r="F52" s="32">
+        <v>1</v>
+      </c>
+      <c r="G52" s="32">
+        <v>0</v>
+      </c>
+      <c r="H52" s="32">
+        <v>0</v>
+      </c>
+      <c r="I52" s="32">
+        <v>0</v>
+      </c>
+      <c r="J52" s="32">
+        <v>54</v>
+      </c>
+      <c r="K52" s="32">
+        <v>77</v>
+      </c>
+      <c r="L52" s="32">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="32">
+        <v>3</v>
+      </c>
+      <c r="C53" s="32">
+        <v>1</v>
+      </c>
+      <c r="D53" s="32">
+        <v>0</v>
+      </c>
+      <c r="E53" s="32">
+        <v>0</v>
+      </c>
+      <c r="F53" s="32">
+        <v>1</v>
+      </c>
+      <c r="G53" s="32">
+        <v>1</v>
+      </c>
+      <c r="H53" s="32">
+        <v>0</v>
+      </c>
+      <c r="I53" s="32">
+        <v>0</v>
+      </c>
+      <c r="J53" s="32">
+        <v>45</v>
+      </c>
+      <c r="K53" s="32">
+        <v>48</v>
+      </c>
+      <c r="L53" s="32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="35">
+        <f>SUM(B2:B53)</f>
+        <v>446</v>
+      </c>
+      <c r="C54" s="35">
+        <f t="shared" ref="C54:L54" si="0">SUM(C2:C53)</f>
+        <v>5</v>
+      </c>
+      <c r="D54" s="35">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E54" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="35">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="G54" s="35">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="H54" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I54" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J54" s="35">
+        <f t="shared" si="0"/>
+        <v>2158</v>
+      </c>
+      <c r="K54" s="35">
+        <f t="shared" si="0"/>
+        <v>2635</v>
+      </c>
+      <c r="L54" s="35">
+        <f t="shared" si="0"/>
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="31"/>
+      <c r="E55" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F55" s="36">
+        <f>G54</f>
+        <v>121</v>
+      </c>
+      <c r="J55">
+        <f>B54-C54</f>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E56" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F56" s="36">
+        <f>B54</f>
+        <v>446</v>
+      </c>
+      <c r="J56">
+        <f>D54-E54</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E57" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F57" s="36">
+        <v>11</v>
+      </c>
+      <c r="J57">
+        <f>F63</f>
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E58" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F58" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F59" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J59" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f>SUM(F55:F59)</f>
+        <v>581</v>
+      </c>
+      <c r="J60">
+        <f>SUM(J55:J59)</f>
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>45</v>
+      </c>
+      <c r="F61">
+        <f>K54-F60</f>
+        <v>2054</v>
+      </c>
+      <c r="J61" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F62" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J62">
+        <f>J60-L54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f>F61+F60</f>
+        <v>2635</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996C5560-3111-494C-AEED-C729859A55D4}">
+  <dimension ref="A1:L61"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
@@ -2191,10 +4528,10 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="B2" s="32">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="32">
         <v>0</v>
@@ -2209,7 +4546,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2" s="32">
         <v>0</v>
@@ -2218,27 +4555,27 @@
         <v>0</v>
       </c>
       <c r="J2" s="32">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K2" s="32">
         <v>50</v>
       </c>
       <c r="L2" s="32">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="B3" s="32">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="32">
         <v>0</v>
       </c>
       <c r="D3" s="32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" s="32">
         <v>0</v>
@@ -2247,7 +4584,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H3" s="32">
         <v>0</v>
@@ -2256,27 +4593,27 @@
         <v>0</v>
       </c>
       <c r="J3" s="32">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K3" s="32">
         <v>50</v>
       </c>
       <c r="L3" s="32">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="B4" s="32">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C4" s="32">
         <v>0</v>
       </c>
       <c r="D4" s="32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4" s="32">
         <v>0</v>
@@ -2285,7 +4622,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="32">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H4" s="32">
         <v>0</v>
@@ -2294,21 +4631,21 @@
         <v>0</v>
       </c>
       <c r="J4" s="32">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="K4" s="32">
         <v>50</v>
       </c>
       <c r="L4" s="32">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B5" s="32">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5" s="32">
         <v>0</v>
@@ -2320,10 +4657,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="32">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5" s="32">
         <v>0</v>
@@ -2332,21 +4669,21 @@
         <v>0</v>
       </c>
       <c r="J5" s="32">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K5" s="32">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="L5" s="32">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="B6" s="32">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C6" s="32">
         <v>0</v>
@@ -2361,7 +4698,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" s="32">
         <v>0</v>
@@ -2370,36 +4707,36 @@
         <v>0</v>
       </c>
       <c r="J6" s="32">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K6" s="32">
         <v>50</v>
       </c>
       <c r="L6" s="32">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="B7" s="32">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C7" s="32">
         <v>0</v>
       </c>
       <c r="D7" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="32">
         <v>0</v>
       </c>
       <c r="F7" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" s="32">
         <v>0</v>
@@ -2408,27 +4745,27 @@
         <v>0</v>
       </c>
       <c r="J7" s="32">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="K7" s="32">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L7" s="32">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="B8" s="32">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="32">
         <v>0</v>
       </c>
       <c r="D8" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="32">
         <v>0</v>
@@ -2437,7 +4774,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H8" s="32">
         <v>0</v>
@@ -2446,21 +4783,21 @@
         <v>0</v>
       </c>
       <c r="J8" s="32">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="K8" s="32">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="L8" s="32">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="B9" s="32">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C9" s="32">
         <v>0</v>
@@ -2475,7 +4812,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9" s="32">
         <v>0</v>
@@ -2484,33 +4821,33 @@
         <v>0</v>
       </c>
       <c r="J9" s="32">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K9" s="32">
         <v>50</v>
       </c>
       <c r="L9" s="32">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="B10" s="32">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C10" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" s="32">
         <v>0</v>
       </c>
       <c r="F10" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="32">
         <v>3</v>
@@ -2522,37 +4859,37 @@
         <v>0</v>
       </c>
       <c r="J10" s="32">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="K10" s="32">
         <v>50</v>
       </c>
       <c r="L10" s="32">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="B11" s="32">
+        <v>8</v>
+      </c>
+      <c r="C11" s="32">
+        <v>0</v>
+      </c>
+      <c r="D11" s="32">
+        <v>0</v>
+      </c>
+      <c r="E11" s="32">
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <v>0</v>
+      </c>
+      <c r="G11" s="32">
         <v>4</v>
       </c>
-      <c r="C11" s="32">
-        <v>0</v>
-      </c>
-      <c r="D11" s="32">
-        <v>0</v>
-      </c>
-      <c r="E11" s="32">
-        <v>0</v>
-      </c>
-      <c r="F11" s="32">
-        <v>1</v>
-      </c>
-      <c r="G11" s="32">
-        <v>1</v>
-      </c>
       <c r="H11" s="32">
         <v>0</v>
       </c>
@@ -2560,21 +4897,21 @@
         <v>0</v>
       </c>
       <c r="J11" s="32">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K11" s="32">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="L11" s="32">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="B12" s="32">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="32">
         <v>0</v>
@@ -2589,7 +4926,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="32">
         <v>0</v>
@@ -2598,21 +4935,21 @@
         <v>0</v>
       </c>
       <c r="J12" s="32">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K12" s="32">
         <v>50</v>
       </c>
       <c r="L12" s="32">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="B13" s="32">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C13" s="32">
         <v>0</v>
@@ -2624,10 +4961,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="32">
         <v>0</v>
@@ -2636,33 +4973,33 @@
         <v>0</v>
       </c>
       <c r="J13" s="32">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="K13" s="32">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="L13" s="32">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="B14" s="32">
         <v>14</v>
       </c>
       <c r="C14" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="32">
         <v>0</v>
       </c>
       <c r="F14" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="32">
         <v>3</v>
@@ -2674,21 +5011,21 @@
         <v>0</v>
       </c>
       <c r="J14" s="32">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="K14" s="32">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="L14" s="32">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="B15" s="32">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C15" s="32">
         <v>0</v>
@@ -2703,7 +5040,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H15" s="32">
         <v>0</v>
@@ -2712,21 +5049,21 @@
         <v>0</v>
       </c>
       <c r="J15" s="32">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="K15" s="32">
         <v>50</v>
       </c>
       <c r="L15" s="32">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="B16" s="32">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C16" s="32">
         <v>0</v>
@@ -2741,7 +5078,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H16" s="32">
         <v>0</v>
@@ -2750,21 +5087,21 @@
         <v>0</v>
       </c>
       <c r="J16" s="32">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="K16" s="32">
         <v>50</v>
       </c>
       <c r="L16" s="32">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>67</v>
+        <v>120</v>
       </c>
       <c r="B17" s="32">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" s="32">
         <v>0</v>
@@ -2779,7 +5116,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H17" s="32">
         <v>0</v>
@@ -2788,27 +5125,27 @@
         <v>0</v>
       </c>
       <c r="J17" s="32">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K17" s="32">
         <v>50</v>
       </c>
       <c r="L17" s="32">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="B18" s="32">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C18" s="32">
         <v>0</v>
       </c>
       <c r="D18" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="32">
         <v>0</v>
@@ -2817,7 +5154,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H18" s="32">
         <v>0</v>
@@ -2826,36 +5163,36 @@
         <v>0</v>
       </c>
       <c r="J18" s="32">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K18" s="32">
         <v>50</v>
       </c>
       <c r="L18" s="32">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="B19" s="32">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C19" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="32">
         <v>0</v>
       </c>
       <c r="F19" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H19" s="32">
         <v>0</v>
@@ -2864,21 +5201,21 @@
         <v>0</v>
       </c>
       <c r="J19" s="32">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="K19" s="32">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="L19" s="32">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
-        <v>70</v>
+        <v>123</v>
       </c>
       <c r="B20" s="32">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C20" s="32">
         <v>0</v>
@@ -2893,7 +5230,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20" s="32">
         <v>0</v>
@@ -2902,24 +5239,24 @@
         <v>0</v>
       </c>
       <c r="J20" s="32">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K20" s="32">
         <v>50</v>
       </c>
       <c r="L20" s="32">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
-        <v>71</v>
+        <v>124</v>
       </c>
       <c r="B21" s="32">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C21" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="32">
         <v>0</v>
@@ -2928,10 +5265,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" s="32">
         <v>0</v>
@@ -2940,24 +5277,24 @@
         <v>0</v>
       </c>
       <c r="J21" s="32">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K21" s="32">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L21" s="32">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
       <c r="B22" s="32">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C22" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="32">
         <v>0</v>
@@ -2966,10 +5303,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H22" s="32">
         <v>0</v>
@@ -2978,21 +5315,21 @@
         <v>0</v>
       </c>
       <c r="J22" s="32">
+        <v>36</v>
+      </c>
+      <c r="K22" s="32">
         <v>49</v>
       </c>
-      <c r="K22" s="32">
-        <v>50</v>
-      </c>
       <c r="L22" s="32">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="B23" s="32">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C23" s="32">
         <v>0</v>
@@ -3007,7 +5344,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H23" s="32">
         <v>0</v>
@@ -3016,21 +5353,21 @@
         <v>0</v>
       </c>
       <c r="J23" s="32">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K23" s="32">
         <v>50</v>
       </c>
       <c r="L23" s="32">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="B24" s="32">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C24" s="32">
         <v>0</v>
@@ -3045,7 +5382,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H24" s="32">
         <v>0</v>
@@ -3054,21 +5391,21 @@
         <v>0</v>
       </c>
       <c r="J24" s="32">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K24" s="32">
         <v>50</v>
       </c>
       <c r="L24" s="32">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
       <c r="B25" s="32">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C25" s="32">
         <v>0</v>
@@ -3083,7 +5420,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H25" s="32">
         <v>0</v>
@@ -3092,18 +5429,18 @@
         <v>0</v>
       </c>
       <c r="J25" s="32">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="K25" s="32">
         <v>50</v>
       </c>
       <c r="L25" s="32">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="B26" s="32">
         <v>5</v>
@@ -3121,7 +5458,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H26" s="32">
         <v>0</v>
@@ -3141,10 +5478,10 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="B27" s="32">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C27" s="32">
         <v>0</v>
@@ -3156,10 +5493,10 @@
         <v>0</v>
       </c>
       <c r="F27" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="32">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H27" s="32">
         <v>0</v>
@@ -3168,18 +5505,18 @@
         <v>0</v>
       </c>
       <c r="J27" s="32">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="K27" s="32">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="L27" s="32">
-        <v>62</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="B28" s="32">
         <v>7</v>
@@ -3188,16 +5525,16 @@
         <v>0</v>
       </c>
       <c r="D28" s="32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E28" s="32">
         <v>0</v>
       </c>
       <c r="F28" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="32">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H28" s="32">
         <v>0</v>
@@ -3206,36 +5543,36 @@
         <v>0</v>
       </c>
       <c r="J28" s="32">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K28" s="32">
         <v>50</v>
       </c>
       <c r="L28" s="32">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="B29" s="32">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C29" s="32">
         <v>0</v>
       </c>
       <c r="D29" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="32">
         <v>0</v>
       </c>
       <c r="F29" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H29" s="32">
         <v>0</v>
@@ -3244,18 +5581,18 @@
         <v>0</v>
       </c>
       <c r="J29" s="32">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="K29" s="32">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="L29" s="32">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="B30" s="32">
         <v>5</v>
@@ -3273,7 +5610,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="32">
         <v>0</v>
@@ -3293,16 +5630,16 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="B31" s="32">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C31" s="32">
         <v>0</v>
       </c>
       <c r="D31" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="32">
         <v>0</v>
@@ -3311,7 +5648,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H31" s="32">
         <v>0</v>
@@ -3320,18 +5657,18 @@
         <v>0</v>
       </c>
       <c r="J31" s="32">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K31" s="32">
         <v>50</v>
       </c>
       <c r="L31" s="32">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="B32" s="32">
         <v>5</v>
@@ -3340,7 +5677,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="32">
         <v>0</v>
@@ -3349,7 +5686,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="32">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H32" s="32">
         <v>0</v>
@@ -3358,36 +5695,36 @@
         <v>0</v>
       </c>
       <c r="J32" s="32">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K32" s="32">
         <v>50</v>
       </c>
       <c r="L32" s="32">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
-        <v>83</v>
+        <v>136</v>
       </c>
       <c r="B33" s="32">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C33" s="32">
         <v>0</v>
       </c>
       <c r="D33" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="32">
         <v>0</v>
       </c>
       <c r="F33" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="32">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H33" s="32">
         <v>0</v>
@@ -3396,36 +5733,36 @@
         <v>0</v>
       </c>
       <c r="J33" s="32">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="K33" s="32">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="L33" s="32">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="B34" s="32">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C34" s="32">
         <v>0</v>
       </c>
       <c r="D34" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="32">
         <v>0</v>
       </c>
       <c r="F34" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H34" s="32">
         <v>0</v>
@@ -3434,36 +5771,36 @@
         <v>0</v>
       </c>
       <c r="J34" s="32">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="K34" s="32">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L34" s="32">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="B35" s="32">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C35" s="32">
         <v>0</v>
       </c>
       <c r="D35" s="32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E35" s="32">
         <v>0</v>
       </c>
       <c r="F35" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" s="32">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H35" s="32">
         <v>0</v>
@@ -3472,36 +5809,36 @@
         <v>0</v>
       </c>
       <c r="J35" s="32">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="K35" s="32">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="L35" s="32">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>86</v>
+        <v>139</v>
       </c>
       <c r="B36" s="32">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C36" s="32">
         <v>0</v>
       </c>
       <c r="D36" s="32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E36" s="32">
         <v>0</v>
       </c>
       <c r="F36" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H36" s="32">
         <v>0</v>
@@ -3510,21 +5847,21 @@
         <v>0</v>
       </c>
       <c r="J36" s="32">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K36" s="32">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L36" s="32">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="B37" s="32">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C37" s="32">
         <v>0</v>
@@ -3536,10 +5873,10 @@
         <v>0</v>
       </c>
       <c r="F37" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="32">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H37" s="32">
         <v>0</v>
@@ -3548,18 +5885,18 @@
         <v>0</v>
       </c>
       <c r="J37" s="32">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K37" s="32">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="L37" s="32">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
-        <v>88</v>
+        <v>141</v>
       </c>
       <c r="B38" s="32">
         <v>7</v>
@@ -3577,7 +5914,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H38" s="32">
         <v>0</v>
@@ -3597,16 +5934,16 @@
     </row>
     <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
-        <v>89</v>
+        <v>142</v>
       </c>
       <c r="B39" s="32">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C39" s="32">
         <v>0</v>
       </c>
       <c r="D39" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" s="32">
         <v>0</v>
@@ -3615,7 +5952,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="32">
         <v>0</v>
@@ -3624,36 +5961,36 @@
         <v>0</v>
       </c>
       <c r="J39" s="32">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="K39" s="32">
         <v>50</v>
       </c>
       <c r="L39" s="32">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>90</v>
+        <v>143</v>
       </c>
       <c r="B40" s="32">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C40" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E40" s="32">
         <v>0</v>
       </c>
       <c r="F40" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" s="32">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H40" s="32">
         <v>0</v>
@@ -3662,21 +5999,21 @@
         <v>0</v>
       </c>
       <c r="J40" s="32">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="K40" s="32">
         <v>50</v>
       </c>
       <c r="L40" s="32">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
       <c r="B41" s="32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C41" s="32">
         <v>1</v>
@@ -3688,10 +6025,10 @@
         <v>0</v>
       </c>
       <c r="F41" s="32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G41" s="32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H41" s="32">
         <v>0</v>
@@ -3700,21 +6037,21 @@
         <v>0</v>
       </c>
       <c r="J41" s="32">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="K41" s="32">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="L41" s="32">
-        <v>82</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="B42" s="32">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C42" s="32">
         <v>0</v>
@@ -3729,7 +6066,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="32">
         <v>0</v>
@@ -3738,21 +6075,21 @@
         <v>0</v>
       </c>
       <c r="J42" s="32">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="K42" s="32">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L42" s="32">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="B43" s="32">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C43" s="32">
         <v>0</v>
@@ -3776,21 +6113,21 @@
         <v>0</v>
       </c>
       <c r="J43" s="32">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="K43" s="32">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="L43" s="32">
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="B44" s="32">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C44" s="32">
         <v>0</v>
@@ -3814,21 +6151,21 @@
         <v>0</v>
       </c>
       <c r="J44" s="32">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K44" s="32">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L44" s="32">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>95</v>
+        <v>148</v>
       </c>
       <c r="B45" s="32">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C45" s="32">
         <v>0</v>
@@ -3852,21 +6189,21 @@
         <v>0</v>
       </c>
       <c r="J45" s="32">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K45" s="32">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L45" s="32">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="B46" s="32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C46" s="32">
         <v>0</v>
@@ -3890,21 +6227,21 @@
         <v>0</v>
       </c>
       <c r="J46" s="32">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="K46" s="32">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="L46" s="32">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
       <c r="B47" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C47" s="32">
         <v>0</v>
@@ -3928,21 +6265,21 @@
         <v>0</v>
       </c>
       <c r="J47" s="32">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="K47" s="32">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="L47" s="32">
-        <v>47</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="B48" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" s="32">
         <v>0</v>
@@ -3954,7 +6291,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="32">
         <v>0</v>
@@ -3966,21 +6303,21 @@
         <v>0</v>
       </c>
       <c r="J48" s="32">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="K48" s="32">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="L48" s="32">
-        <v>52</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="B49" s="32">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C49" s="32">
         <v>0</v>
@@ -3992,33 +6329,33 @@
         <v>0</v>
       </c>
       <c r="F49" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G49" s="32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H49" s="32">
         <v>0</v>
       </c>
       <c r="I49" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" s="32">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="K49" s="32">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="L49" s="32">
-        <v>53</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
       <c r="B50" s="32">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C50" s="32">
         <v>0</v>
@@ -4030,7 +6367,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="32">
         <v>0</v>
@@ -4042,21 +6379,21 @@
         <v>0</v>
       </c>
       <c r="J50" s="32">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K50" s="32">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="L50" s="32">
-        <v>69</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="B51" s="32">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C51" s="32">
         <v>0</v>
@@ -4068,7 +6405,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="32">
         <v>0</v>
@@ -4080,230 +6417,153 @@
         <v>0</v>
       </c>
       <c r="J51" s="32">
+        <v>28</v>
+      </c>
+      <c r="K51" s="32">
+        <v>38</v>
+      </c>
+      <c r="L51" s="32">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B52" s="35">
+        <f>SUM(B2:B51)</f>
+        <v>492</v>
+      </c>
+      <c r="C52" s="35">
+        <f t="shared" ref="C52:L52" si="0">SUM(C2:C51)</f>
+        <v>4</v>
+      </c>
+      <c r="D52" s="35">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E52" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="35">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G52" s="35">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="H52" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="35">
+        <f t="shared" si="0"/>
+        <v>1795</v>
+      </c>
+      <c r="K52" s="35">
+        <f t="shared" si="0"/>
+        <v>2330</v>
+      </c>
+      <c r="L52" s="35">
+        <f t="shared" si="0"/>
+        <v>2845</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E53" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F53" s="36">
+        <f>G52</f>
+        <v>105</v>
+      </c>
+      <c r="J53">
+        <f>B52-C52</f>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E54" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="K51" s="32">
-        <v>50</v>
-      </c>
-      <c r="L51" s="32">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="32">
-        <v>22</v>
-      </c>
-      <c r="C52" s="32">
-        <v>0</v>
-      </c>
-      <c r="D52" s="32">
-        <v>0</v>
-      </c>
-      <c r="E52" s="32">
-        <v>0</v>
-      </c>
-      <c r="F52" s="32">
-        <v>1</v>
-      </c>
-      <c r="G52" s="32">
-        <v>0</v>
-      </c>
-      <c r="H52" s="32">
-        <v>0</v>
-      </c>
-      <c r="I52" s="32">
-        <v>0</v>
-      </c>
-      <c r="J52" s="32">
-        <v>54</v>
-      </c>
-      <c r="K52" s="32">
-        <v>77</v>
-      </c>
-      <c r="L52" s="32">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="B53" s="32">
-        <v>3</v>
-      </c>
-      <c r="C53" s="32">
-        <v>1</v>
-      </c>
-      <c r="D53" s="32">
-        <v>0</v>
-      </c>
-      <c r="E53" s="32">
-        <v>0</v>
-      </c>
-      <c r="F53" s="32">
-        <v>1</v>
-      </c>
-      <c r="G53" s="32">
-        <v>1</v>
-      </c>
-      <c r="H53" s="32">
-        <v>0</v>
-      </c>
-      <c r="I53" s="32">
-        <v>0</v>
-      </c>
-      <c r="J53" s="32">
-        <v>45</v>
-      </c>
-      <c r="K53" s="32">
-        <v>48</v>
-      </c>
-      <c r="L53" s="32">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="B54" s="35">
-        <f>SUM(B2:B53)</f>
-        <v>446</v>
-      </c>
-      <c r="C54" s="35">
-        <f t="shared" ref="C54:L54" si="0">SUM(C2:C53)</f>
-        <v>5</v>
-      </c>
-      <c r="D54" s="35">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="E54" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="35">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="G54" s="35">
-        <f t="shared" si="0"/>
-        <v>121</v>
-      </c>
-      <c r="H54" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I54" s="35">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J54" s="35">
-        <f t="shared" si="0"/>
-        <v>2158</v>
-      </c>
-      <c r="K54" s="35">
-        <f t="shared" si="0"/>
-        <v>2635</v>
-      </c>
-      <c r="L54" s="35">
-        <f t="shared" si="0"/>
-        <v>3088</v>
+      <c r="F54" s="36">
+        <f>B52</f>
+        <v>492</v>
+      </c>
+      <c r="J54">
+        <f>D52-E52</f>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="31"/>
       <c r="E55" s="36" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F55" s="36">
-        <f>G54</f>
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="J55">
-        <f>B54-C54</f>
-        <v>441</v>
+        <f>F61</f>
+        <v>2330</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E56" s="36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F56" s="36">
-        <f>B54</f>
-        <v>446</v>
-      </c>
-      <c r="J56">
-        <f>D54-E54</f>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E57" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="F57" s="36">
-        <v>11</v>
-      </c>
-      <c r="J57">
-        <f>F63</f>
-        <v>2635</v>
+      <c r="F57" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J57" s="34" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E58" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F58" s="36">
-        <v>3</v>
+      <c r="F58">
+        <f>SUM(F53:F57)</f>
+        <v>624</v>
+      </c>
+      <c r="J58">
+        <f>SUM(J53:J57)</f>
+        <v>2845</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F59" s="34" t="s">
+      <c r="E59" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59">
+        <f>K52-F58</f>
+        <v>1706</v>
+      </c>
+      <c r="J59" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F60" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="J59" s="34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F60">
-        <f>SUM(F55:F59)</f>
-        <v>581</v>
-      </c>
       <c r="J60">
-        <f>SUM(J55:J59)</f>
-        <v>3088</v>
+        <f>J58-L52</f>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E61" t="s">
-        <v>45</v>
-      </c>
       <c r="F61">
-        <f>K54-F60</f>
-        <v>2054</v>
-      </c>
-      <c r="J61" s="34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F62" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="J62">
-        <f>J60-L54</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F63">
-        <f>F61+F60</f>
-        <v>2635</v>
+        <f>F59+F58</f>
+        <v>2330</v>
       </c>
     </row>
   </sheetData>
@@ -4311,7 +6571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:J31"/>
   <sheetViews>
@@ -4357,7 +6617,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="114.75" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
nmv 18 04 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 7.1 TO 7.5.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 7.1 TO 7.5.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772E04F1-B983-44F5-AFD8-1D36EB35CBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEEF83B-1E79-4608-AF96-A1887BAA85F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="7.1" sheetId="15" r:id="rId1"/>
     <sheet name="7.2" sheetId="16" r:id="rId2"/>
-    <sheet name="total 7.1 to 7.5" sheetId="7" r:id="rId3"/>
+    <sheet name="7.3" sheetId="17" r:id="rId3"/>
+    <sheet name="total 7.1 to 7.5" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="199">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1700,6 +1701,135 @@
   </si>
   <si>
     <t>50</t>
+  </si>
+  <si>
+    <t>7.3.1.1 :</t>
+  </si>
+  <si>
+    <t>7.3.1.2 :</t>
+  </si>
+  <si>
+    <t>7.3.1.3 :</t>
+  </si>
+  <si>
+    <t>7.3.1.4 :</t>
+  </si>
+  <si>
+    <t>7.3.2.1 :</t>
+  </si>
+  <si>
+    <t>7.3.2.2 :</t>
+  </si>
+  <si>
+    <t>7.3.3.1 :</t>
+  </si>
+  <si>
+    <t>7.3.3.2 :</t>
+  </si>
+  <si>
+    <t>7.3.4.1 :</t>
+  </si>
+  <si>
+    <t>7.3.4.2 :</t>
+  </si>
+  <si>
+    <t>7.3.5.1 :</t>
+  </si>
+  <si>
+    <t>7.3.5.2 :</t>
+  </si>
+  <si>
+    <t>7.3.5.3 :</t>
+  </si>
+  <si>
+    <t>7.3.6.1 :</t>
+  </si>
+  <si>
+    <t>7.3.6.2 :</t>
+  </si>
+  <si>
+    <t>7.3.7.1 :</t>
+  </si>
+  <si>
+    <t>7.3.7.2 :</t>
+  </si>
+  <si>
+    <t>7.3.7.3 :</t>
+  </si>
+  <si>
+    <t>7.3.7.4 :</t>
+  </si>
+  <si>
+    <t>7.3.8.1 :</t>
+  </si>
+  <si>
+    <t>7.3.8.2 :</t>
+  </si>
+  <si>
+    <t>7.3.9.1 :</t>
+  </si>
+  <si>
+    <t>7.3.9.2 :</t>
+  </si>
+  <si>
+    <t>7.3.9.3 :</t>
+  </si>
+  <si>
+    <t>7.3.10.1 :</t>
+  </si>
+  <si>
+    <t>7.3.10.2 :</t>
+  </si>
+  <si>
+    <t>7.3.10.3 :</t>
+  </si>
+  <si>
+    <t>7.3.10.4 :</t>
+  </si>
+  <si>
+    <t>7.3.10.5 :</t>
+  </si>
+  <si>
+    <t>7.3.11.1 :</t>
+  </si>
+  <si>
+    <t>7.3.11.2 :</t>
+  </si>
+  <si>
+    <t>7.3.11.3 :</t>
+  </si>
+  <si>
+    <t>7.3.12.1 :</t>
+  </si>
+  <si>
+    <t>7.3.13.1 :</t>
+  </si>
+  <si>
+    <t>7.3.14.1 :</t>
+  </si>
+  <si>
+    <t>7.3.15.1 :</t>
+  </si>
+  <si>
+    <t>7.3.16.1 :</t>
+  </si>
+  <si>
+    <t>7.3.16.2 :</t>
+  </si>
+  <si>
+    <t>7.3.17.1 :</t>
+  </si>
+  <si>
+    <t>7.3.18.1 :</t>
+  </si>
+  <si>
+    <t>7.3.19.1 :</t>
+  </si>
+  <si>
+    <t>7.3.20.1 :</t>
+  </si>
+  <si>
+    <t>42</t>
   </si>
 </sst>
 </file>
@@ -4469,9 +4599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996C5560-3111-494C-AEED-C729859A55D4}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53:J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6572,6 +6702,1808 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7653A96A-DC13-412E-A625-399CF21DC8FF}">
+  <dimension ref="A1:L53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44:L44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="32">
+        <v>11</v>
+      </c>
+      <c r="C2" s="32">
+        <v>0</v>
+      </c>
+      <c r="D2" s="32">
+        <v>0</v>
+      </c>
+      <c r="E2" s="32">
+        <v>0</v>
+      </c>
+      <c r="F2" s="32">
+        <v>0</v>
+      </c>
+      <c r="G2" s="32">
+        <v>1</v>
+      </c>
+      <c r="H2" s="32">
+        <v>0</v>
+      </c>
+      <c r="I2" s="32">
+        <v>0</v>
+      </c>
+      <c r="J2" s="32">
+        <v>39</v>
+      </c>
+      <c r="K2" s="32">
+        <v>50</v>
+      </c>
+      <c r="L2" s="32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="32">
+        <v>10</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0</v>
+      </c>
+      <c r="D3" s="32">
+        <v>1</v>
+      </c>
+      <c r="E3" s="32">
+        <v>0</v>
+      </c>
+      <c r="F3" s="32">
+        <v>0</v>
+      </c>
+      <c r="G3" s="32">
+        <v>2</v>
+      </c>
+      <c r="H3" s="32">
+        <v>0</v>
+      </c>
+      <c r="I3" s="32">
+        <v>0</v>
+      </c>
+      <c r="J3" s="32">
+        <v>39</v>
+      </c>
+      <c r="K3" s="32">
+        <v>50</v>
+      </c>
+      <c r="L3" s="32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="32">
+        <v>8</v>
+      </c>
+      <c r="C4" s="32">
+        <v>0</v>
+      </c>
+      <c r="D4" s="32">
+        <v>0</v>
+      </c>
+      <c r="E4" s="32">
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <v>0</v>
+      </c>
+      <c r="G4" s="32">
+        <v>1</v>
+      </c>
+      <c r="H4" s="32">
+        <v>0</v>
+      </c>
+      <c r="I4" s="32">
+        <v>0</v>
+      </c>
+      <c r="J4" s="32">
+        <v>42</v>
+      </c>
+      <c r="K4" s="32">
+        <v>50</v>
+      </c>
+      <c r="L4" s="32">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="32">
+        <v>11</v>
+      </c>
+      <c r="C5" s="32">
+        <v>1</v>
+      </c>
+      <c r="D5" s="32">
+        <v>0</v>
+      </c>
+      <c r="E5" s="32">
+        <v>0</v>
+      </c>
+      <c r="F5" s="32">
+        <v>1</v>
+      </c>
+      <c r="G5" s="32">
+        <v>2</v>
+      </c>
+      <c r="H5" s="32">
+        <v>0</v>
+      </c>
+      <c r="I5" s="32">
+        <v>0</v>
+      </c>
+      <c r="J5" s="32">
+        <v>40</v>
+      </c>
+      <c r="K5" s="32">
+        <v>51</v>
+      </c>
+      <c r="L5" s="32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="32">
+        <v>7</v>
+      </c>
+      <c r="C6" s="32">
+        <v>0</v>
+      </c>
+      <c r="D6" s="32">
+        <v>0</v>
+      </c>
+      <c r="E6" s="32">
+        <v>0</v>
+      </c>
+      <c r="F6" s="32">
+        <v>0</v>
+      </c>
+      <c r="G6" s="32">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32">
+        <v>0</v>
+      </c>
+      <c r="I6" s="32">
+        <v>0</v>
+      </c>
+      <c r="J6" s="32">
+        <v>43</v>
+      </c>
+      <c r="K6" s="32">
+        <v>50</v>
+      </c>
+      <c r="L6" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="32">
+        <v>6</v>
+      </c>
+      <c r="C7" s="32">
+        <v>0</v>
+      </c>
+      <c r="D7" s="32">
+        <v>0</v>
+      </c>
+      <c r="E7" s="32">
+        <v>0</v>
+      </c>
+      <c r="F7" s="32">
+        <v>1</v>
+      </c>
+      <c r="G7" s="32">
+        <v>0</v>
+      </c>
+      <c r="H7" s="32">
+        <v>0</v>
+      </c>
+      <c r="I7" s="32">
+        <v>0</v>
+      </c>
+      <c r="J7" s="32">
+        <v>34</v>
+      </c>
+      <c r="K7" s="32">
+        <v>41</v>
+      </c>
+      <c r="L7" s="32">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="32">
+        <v>13</v>
+      </c>
+      <c r="C8" s="32">
+        <v>0</v>
+      </c>
+      <c r="D8" s="32">
+        <v>0</v>
+      </c>
+      <c r="E8" s="32">
+        <v>0</v>
+      </c>
+      <c r="F8" s="32">
+        <v>0</v>
+      </c>
+      <c r="G8" s="32">
+        <v>1</v>
+      </c>
+      <c r="H8" s="32">
+        <v>0</v>
+      </c>
+      <c r="I8" s="32">
+        <v>0</v>
+      </c>
+      <c r="J8" s="32">
+        <v>37</v>
+      </c>
+      <c r="K8" s="32">
+        <v>50</v>
+      </c>
+      <c r="L8" s="32">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="32">
+        <v>14</v>
+      </c>
+      <c r="C9" s="32">
+        <v>0</v>
+      </c>
+      <c r="D9" s="32">
+        <v>0</v>
+      </c>
+      <c r="E9" s="32">
+        <v>0</v>
+      </c>
+      <c r="F9" s="32">
+        <v>1</v>
+      </c>
+      <c r="G9" s="32">
+        <v>3</v>
+      </c>
+      <c r="H9" s="32">
+        <v>0</v>
+      </c>
+      <c r="I9" s="32">
+        <v>0</v>
+      </c>
+      <c r="J9" s="32">
+        <v>28</v>
+      </c>
+      <c r="K9" s="32">
+        <v>43</v>
+      </c>
+      <c r="L9" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" s="32">
+        <v>4</v>
+      </c>
+      <c r="C10" s="32">
+        <v>0</v>
+      </c>
+      <c r="D10" s="32">
+        <v>0</v>
+      </c>
+      <c r="E10" s="32">
+        <v>0</v>
+      </c>
+      <c r="F10" s="32">
+        <v>0</v>
+      </c>
+      <c r="G10" s="32">
+        <v>1</v>
+      </c>
+      <c r="H10" s="32">
+        <v>0</v>
+      </c>
+      <c r="I10" s="32">
+        <v>0</v>
+      </c>
+      <c r="J10" s="32">
+        <v>46</v>
+      </c>
+      <c r="K10" s="32">
+        <v>50</v>
+      </c>
+      <c r="L10" s="32">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="32">
+        <v>6</v>
+      </c>
+      <c r="C11" s="32">
+        <v>1</v>
+      </c>
+      <c r="D11" s="32">
+        <v>0</v>
+      </c>
+      <c r="E11" s="32">
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <v>1</v>
+      </c>
+      <c r="G11" s="32">
+        <v>2</v>
+      </c>
+      <c r="H11" s="32">
+        <v>0</v>
+      </c>
+      <c r="I11" s="32">
+        <v>0</v>
+      </c>
+      <c r="J11" s="32">
+        <v>28</v>
+      </c>
+      <c r="K11" s="32">
+        <v>34</v>
+      </c>
+      <c r="L11" s="32">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="32">
+        <v>8</v>
+      </c>
+      <c r="C12" s="32">
+        <v>0</v>
+      </c>
+      <c r="D12" s="32">
+        <v>0</v>
+      </c>
+      <c r="E12" s="32">
+        <v>0</v>
+      </c>
+      <c r="F12" s="32">
+        <v>0</v>
+      </c>
+      <c r="G12" s="32">
+        <v>5</v>
+      </c>
+      <c r="H12" s="32">
+        <v>0</v>
+      </c>
+      <c r="I12" s="32">
+        <v>0</v>
+      </c>
+      <c r="J12" s="32">
+        <v>42</v>
+      </c>
+      <c r="K12" s="32">
+        <v>50</v>
+      </c>
+      <c r="L12" s="32">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="32">
+        <v>6</v>
+      </c>
+      <c r="C13" s="32">
+        <v>0</v>
+      </c>
+      <c r="D13" s="32">
+        <v>0</v>
+      </c>
+      <c r="E13" s="32">
+        <v>0</v>
+      </c>
+      <c r="F13" s="32">
+        <v>0</v>
+      </c>
+      <c r="G13" s="32">
+        <v>0</v>
+      </c>
+      <c r="H13" s="32">
+        <v>0</v>
+      </c>
+      <c r="I13" s="32">
+        <v>0</v>
+      </c>
+      <c r="J13" s="32">
+        <v>44</v>
+      </c>
+      <c r="K13" s="32">
+        <v>50</v>
+      </c>
+      <c r="L13" s="32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="32">
+        <v>17</v>
+      </c>
+      <c r="C14" s="32">
+        <v>1</v>
+      </c>
+      <c r="D14" s="32">
+        <v>5</v>
+      </c>
+      <c r="E14" s="32">
+        <v>0</v>
+      </c>
+      <c r="F14" s="32">
+        <v>1</v>
+      </c>
+      <c r="G14" s="32">
+        <v>4</v>
+      </c>
+      <c r="H14" s="32">
+        <v>0</v>
+      </c>
+      <c r="I14" s="32">
+        <v>0</v>
+      </c>
+      <c r="J14" s="32">
+        <v>59</v>
+      </c>
+      <c r="K14" s="32">
+        <v>81</v>
+      </c>
+      <c r="L14" s="32">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="32">
+        <v>8</v>
+      </c>
+      <c r="C15" s="32">
+        <v>0</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0</v>
+      </c>
+      <c r="E15" s="32">
+        <v>0</v>
+      </c>
+      <c r="F15" s="32">
+        <v>0</v>
+      </c>
+      <c r="G15" s="32">
+        <v>3</v>
+      </c>
+      <c r="H15" s="32">
+        <v>0</v>
+      </c>
+      <c r="I15" s="32">
+        <v>0</v>
+      </c>
+      <c r="J15" s="32">
+        <v>42</v>
+      </c>
+      <c r="K15" s="32">
+        <v>50</v>
+      </c>
+      <c r="L15" s="32">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="32">
+        <v>8</v>
+      </c>
+      <c r="C16" s="32">
+        <v>1</v>
+      </c>
+      <c r="D16" s="32">
+        <v>0</v>
+      </c>
+      <c r="E16" s="32">
+        <v>0</v>
+      </c>
+      <c r="F16" s="32">
+        <v>1</v>
+      </c>
+      <c r="G16" s="32">
+        <v>4</v>
+      </c>
+      <c r="H16" s="32">
+        <v>0</v>
+      </c>
+      <c r="I16" s="32">
+        <v>0</v>
+      </c>
+      <c r="J16" s="32">
+        <v>43</v>
+      </c>
+      <c r="K16" s="32">
+        <v>51</v>
+      </c>
+      <c r="L16" s="32">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="32">
+        <v>11</v>
+      </c>
+      <c r="C17" s="32">
+        <v>0</v>
+      </c>
+      <c r="D17" s="32">
+        <v>0</v>
+      </c>
+      <c r="E17" s="32">
+        <v>0</v>
+      </c>
+      <c r="F17" s="32">
+        <v>0</v>
+      </c>
+      <c r="G17" s="32">
+        <v>4</v>
+      </c>
+      <c r="H17" s="32">
+        <v>0</v>
+      </c>
+      <c r="I17" s="32">
+        <v>0</v>
+      </c>
+      <c r="J17" s="32">
+        <v>39</v>
+      </c>
+      <c r="K17" s="32">
+        <v>50</v>
+      </c>
+      <c r="L17" s="32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="32">
+        <v>15</v>
+      </c>
+      <c r="C18" s="32">
+        <v>0</v>
+      </c>
+      <c r="D18" s="32">
+        <v>0</v>
+      </c>
+      <c r="E18" s="32">
+        <v>0</v>
+      </c>
+      <c r="F18" s="32">
+        <v>0</v>
+      </c>
+      <c r="G18" s="32">
+        <v>2</v>
+      </c>
+      <c r="H18" s="32">
+        <v>0</v>
+      </c>
+      <c r="I18" s="32">
+        <v>0</v>
+      </c>
+      <c r="J18" s="32">
+        <v>35</v>
+      </c>
+      <c r="K18" s="32">
+        <v>50</v>
+      </c>
+      <c r="L18" s="32">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="32">
+        <v>6</v>
+      </c>
+      <c r="C19" s="32">
+        <v>0</v>
+      </c>
+      <c r="D19" s="32">
+        <v>4</v>
+      </c>
+      <c r="E19" s="32">
+        <v>0</v>
+      </c>
+      <c r="F19" s="32">
+        <v>0</v>
+      </c>
+      <c r="G19" s="32">
+        <v>1</v>
+      </c>
+      <c r="H19" s="32">
+        <v>0</v>
+      </c>
+      <c r="I19" s="32">
+        <v>0</v>
+      </c>
+      <c r="J19" s="32">
+        <v>40</v>
+      </c>
+      <c r="K19" s="32">
+        <v>50</v>
+      </c>
+      <c r="L19" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" s="32">
+        <v>15</v>
+      </c>
+      <c r="C20" s="32">
+        <v>1</v>
+      </c>
+      <c r="D20" s="32">
+        <v>1</v>
+      </c>
+      <c r="E20" s="32">
+        <v>0</v>
+      </c>
+      <c r="F20" s="32">
+        <v>1</v>
+      </c>
+      <c r="G20" s="32">
+        <v>3</v>
+      </c>
+      <c r="H20" s="32">
+        <v>0</v>
+      </c>
+      <c r="I20" s="32">
+        <v>0</v>
+      </c>
+      <c r="J20" s="32">
+        <v>36</v>
+      </c>
+      <c r="K20" s="32">
+        <v>52</v>
+      </c>
+      <c r="L20" s="32">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="32">
+        <v>10</v>
+      </c>
+      <c r="C21" s="32">
+        <v>0</v>
+      </c>
+      <c r="D21" s="32">
+        <v>1</v>
+      </c>
+      <c r="E21" s="32">
+        <v>0</v>
+      </c>
+      <c r="F21" s="32">
+        <v>0</v>
+      </c>
+      <c r="G21" s="32">
+        <v>3</v>
+      </c>
+      <c r="H21" s="32">
+        <v>0</v>
+      </c>
+      <c r="I21" s="32">
+        <v>0</v>
+      </c>
+      <c r="J21" s="32">
+        <v>39</v>
+      </c>
+      <c r="K21" s="32">
+        <v>50</v>
+      </c>
+      <c r="L21" s="32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="32">
+        <v>11</v>
+      </c>
+      <c r="C22" s="32">
+        <v>1</v>
+      </c>
+      <c r="D22" s="32">
+        <v>0</v>
+      </c>
+      <c r="E22" s="32">
+        <v>0</v>
+      </c>
+      <c r="F22" s="32">
+        <v>1</v>
+      </c>
+      <c r="G22" s="32">
+        <v>2</v>
+      </c>
+      <c r="H22" s="32">
+        <v>0</v>
+      </c>
+      <c r="I22" s="32">
+        <v>0</v>
+      </c>
+      <c r="J22" s="32">
+        <v>26</v>
+      </c>
+      <c r="K22" s="32">
+        <v>37</v>
+      </c>
+      <c r="L22" s="32">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="32">
+        <v>4</v>
+      </c>
+      <c r="C23" s="32">
+        <v>0</v>
+      </c>
+      <c r="D23" s="32">
+        <v>0</v>
+      </c>
+      <c r="E23" s="32">
+        <v>0</v>
+      </c>
+      <c r="F23" s="32">
+        <v>0</v>
+      </c>
+      <c r="G23" s="32">
+        <v>3</v>
+      </c>
+      <c r="H23" s="32">
+        <v>0</v>
+      </c>
+      <c r="I23" s="32">
+        <v>0</v>
+      </c>
+      <c r="J23" s="32">
+        <v>46</v>
+      </c>
+      <c r="K23" s="32">
+        <v>50</v>
+      </c>
+      <c r="L23" s="32">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" s="32">
+        <v>9</v>
+      </c>
+      <c r="C24" s="32">
+        <v>0</v>
+      </c>
+      <c r="D24" s="32">
+        <v>2</v>
+      </c>
+      <c r="E24" s="32">
+        <v>0</v>
+      </c>
+      <c r="F24" s="32">
+        <v>0</v>
+      </c>
+      <c r="G24" s="32">
+        <v>2</v>
+      </c>
+      <c r="H24" s="32">
+        <v>0</v>
+      </c>
+      <c r="I24" s="32">
+        <v>0</v>
+      </c>
+      <c r="J24" s="32">
+        <v>39</v>
+      </c>
+      <c r="K24" s="32">
+        <v>50</v>
+      </c>
+      <c r="L24" s="32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25" s="32">
+        <v>16</v>
+      </c>
+      <c r="C25" s="32">
+        <v>1</v>
+      </c>
+      <c r="D25" s="32">
+        <v>5</v>
+      </c>
+      <c r="E25" s="32">
+        <v>0</v>
+      </c>
+      <c r="F25" s="32">
+        <v>1</v>
+      </c>
+      <c r="G25" s="32">
+        <v>2</v>
+      </c>
+      <c r="H25" s="32">
+        <v>0</v>
+      </c>
+      <c r="I25" s="32">
+        <v>0</v>
+      </c>
+      <c r="J25" s="32">
+        <v>52</v>
+      </c>
+      <c r="K25" s="32">
+        <v>73</v>
+      </c>
+      <c r="L25" s="32">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26" s="32">
+        <v>8</v>
+      </c>
+      <c r="C26" s="32">
+        <v>0</v>
+      </c>
+      <c r="D26" s="32">
+        <v>0</v>
+      </c>
+      <c r="E26" s="32">
+        <v>0</v>
+      </c>
+      <c r="F26" s="32">
+        <v>0</v>
+      </c>
+      <c r="G26" s="32">
+        <v>4</v>
+      </c>
+      <c r="H26" s="32">
+        <v>0</v>
+      </c>
+      <c r="I26" s="32">
+        <v>0</v>
+      </c>
+      <c r="J26" s="32">
+        <v>42</v>
+      </c>
+      <c r="K26" s="32">
+        <v>50</v>
+      </c>
+      <c r="L26" s="32">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27" s="32">
+        <v>13</v>
+      </c>
+      <c r="C27" s="32">
+        <v>0</v>
+      </c>
+      <c r="D27" s="32">
+        <v>0</v>
+      </c>
+      <c r="E27" s="32">
+        <v>0</v>
+      </c>
+      <c r="F27" s="32">
+        <v>0</v>
+      </c>
+      <c r="G27" s="32">
+        <v>5</v>
+      </c>
+      <c r="H27" s="32">
+        <v>0</v>
+      </c>
+      <c r="I27" s="32">
+        <v>0</v>
+      </c>
+      <c r="J27" s="32">
+        <v>37</v>
+      </c>
+      <c r="K27" s="32">
+        <v>50</v>
+      </c>
+      <c r="L27" s="32">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="B28" s="32">
+        <v>8</v>
+      </c>
+      <c r="C28" s="32">
+        <v>0</v>
+      </c>
+      <c r="D28" s="32">
+        <v>2</v>
+      </c>
+      <c r="E28" s="32">
+        <v>0</v>
+      </c>
+      <c r="F28" s="32">
+        <v>0</v>
+      </c>
+      <c r="G28" s="32">
+        <v>1</v>
+      </c>
+      <c r="H28" s="32">
+        <v>0</v>
+      </c>
+      <c r="I28" s="32">
+        <v>0</v>
+      </c>
+      <c r="J28" s="32">
+        <v>40</v>
+      </c>
+      <c r="K28" s="32">
+        <v>50</v>
+      </c>
+      <c r="L28" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" s="32">
+        <v>8</v>
+      </c>
+      <c r="C29" s="32">
+        <v>0</v>
+      </c>
+      <c r="D29" s="32">
+        <v>1</v>
+      </c>
+      <c r="E29" s="32">
+        <v>0</v>
+      </c>
+      <c r="F29" s="32">
+        <v>0</v>
+      </c>
+      <c r="G29" s="32">
+        <v>7</v>
+      </c>
+      <c r="H29" s="32">
+        <v>0</v>
+      </c>
+      <c r="I29" s="32">
+        <v>0</v>
+      </c>
+      <c r="J29" s="32">
+        <v>41</v>
+      </c>
+      <c r="K29" s="32">
+        <v>50</v>
+      </c>
+      <c r="L29" s="32">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" s="32">
+        <v>15</v>
+      </c>
+      <c r="C30" s="32">
+        <v>1</v>
+      </c>
+      <c r="D30" s="32">
+        <v>1</v>
+      </c>
+      <c r="E30" s="32">
+        <v>0</v>
+      </c>
+      <c r="F30" s="32">
+        <v>1</v>
+      </c>
+      <c r="G30" s="32">
+        <v>5</v>
+      </c>
+      <c r="H30" s="32">
+        <v>0</v>
+      </c>
+      <c r="I30" s="32">
+        <v>0</v>
+      </c>
+      <c r="J30" s="32">
+        <v>55</v>
+      </c>
+      <c r="K30" s="32">
+        <v>71</v>
+      </c>
+      <c r="L30" s="32">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="32">
+        <v>5</v>
+      </c>
+      <c r="C31" s="32">
+        <v>1</v>
+      </c>
+      <c r="D31" s="32">
+        <v>0</v>
+      </c>
+      <c r="E31" s="32">
+        <v>0</v>
+      </c>
+      <c r="F31" s="32">
+        <v>6</v>
+      </c>
+      <c r="G31" s="32">
+        <v>5</v>
+      </c>
+      <c r="H31" s="32">
+        <v>0</v>
+      </c>
+      <c r="I31" s="32">
+        <v>0</v>
+      </c>
+      <c r="J31" s="32">
+        <v>40</v>
+      </c>
+      <c r="K31" s="32">
+        <v>50</v>
+      </c>
+      <c r="L31" s="32">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32" s="32">
+        <v>15</v>
+      </c>
+      <c r="C32" s="32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="32">
+        <v>6</v>
+      </c>
+      <c r="G32" s="32">
+        <v>6</v>
+      </c>
+      <c r="H32" s="32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="32">
+        <v>0</v>
+      </c>
+      <c r="J32" s="32">
+        <v>30</v>
+      </c>
+      <c r="K32" s="32">
+        <v>50</v>
+      </c>
+      <c r="L32" s="32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="32">
+        <v>5</v>
+      </c>
+      <c r="C33" s="32">
+        <v>0</v>
+      </c>
+      <c r="D33" s="32">
+        <v>0</v>
+      </c>
+      <c r="E33" s="32">
+        <v>0</v>
+      </c>
+      <c r="F33" s="32">
+        <v>4</v>
+      </c>
+      <c r="G33" s="32">
+        <v>5</v>
+      </c>
+      <c r="H33" s="32">
+        <v>0</v>
+      </c>
+      <c r="I33" s="32">
+        <v>0</v>
+      </c>
+      <c r="J33" s="32">
+        <v>23</v>
+      </c>
+      <c r="K33" s="32">
+        <v>32</v>
+      </c>
+      <c r="L33" s="32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="B34" s="32">
+        <v>3</v>
+      </c>
+      <c r="C34" s="32">
+        <v>0</v>
+      </c>
+      <c r="D34" s="32">
+        <v>0</v>
+      </c>
+      <c r="E34" s="32">
+        <v>0</v>
+      </c>
+      <c r="F34" s="32">
+        <v>1</v>
+      </c>
+      <c r="G34" s="32">
+        <v>0</v>
+      </c>
+      <c r="H34" s="32">
+        <v>0</v>
+      </c>
+      <c r="I34" s="32">
+        <v>0</v>
+      </c>
+      <c r="J34" s="32">
+        <v>50</v>
+      </c>
+      <c r="K34" s="32">
+        <v>54</v>
+      </c>
+      <c r="L34" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" s="32">
+        <v>8</v>
+      </c>
+      <c r="C35" s="32">
+        <v>2</v>
+      </c>
+      <c r="D35" s="32">
+        <v>2</v>
+      </c>
+      <c r="E35" s="32">
+        <v>1</v>
+      </c>
+      <c r="F35" s="32">
+        <v>6</v>
+      </c>
+      <c r="G35" s="32">
+        <v>13</v>
+      </c>
+      <c r="H35" s="32">
+        <v>0</v>
+      </c>
+      <c r="I35" s="32">
+        <v>0</v>
+      </c>
+      <c r="J35" s="32">
+        <v>55</v>
+      </c>
+      <c r="K35" s="32">
+        <v>68</v>
+      </c>
+      <c r="L35" s="32">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="B36" s="32">
+        <v>2</v>
+      </c>
+      <c r="C36" s="32">
+        <v>0</v>
+      </c>
+      <c r="D36" s="32">
+        <v>0</v>
+      </c>
+      <c r="E36" s="32">
+        <v>0</v>
+      </c>
+      <c r="F36" s="32">
+        <v>1</v>
+      </c>
+      <c r="G36" s="32">
+        <v>1</v>
+      </c>
+      <c r="H36" s="32">
+        <v>0</v>
+      </c>
+      <c r="I36" s="32">
+        <v>0</v>
+      </c>
+      <c r="J36" s="32">
+        <v>48</v>
+      </c>
+      <c r="K36" s="32">
+        <v>51</v>
+      </c>
+      <c r="L36" s="32">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="B37" s="32">
+        <v>9</v>
+      </c>
+      <c r="C37" s="32">
+        <v>0</v>
+      </c>
+      <c r="D37" s="32">
+        <v>0</v>
+      </c>
+      <c r="E37" s="32">
+        <v>0</v>
+      </c>
+      <c r="F37" s="32">
+        <v>1</v>
+      </c>
+      <c r="G37" s="32">
+        <v>0</v>
+      </c>
+      <c r="H37" s="32">
+        <v>0</v>
+      </c>
+      <c r="I37" s="32">
+        <v>0</v>
+      </c>
+      <c r="J37" s="32">
+        <v>50</v>
+      </c>
+      <c r="K37" s="32">
+        <v>60</v>
+      </c>
+      <c r="L37" s="32">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B38" s="32">
+        <v>5</v>
+      </c>
+      <c r="C38" s="32">
+        <v>0</v>
+      </c>
+      <c r="D38" s="32">
+        <v>0</v>
+      </c>
+      <c r="E38" s="32">
+        <v>0</v>
+      </c>
+      <c r="F38" s="32">
+        <v>0</v>
+      </c>
+      <c r="G38" s="32">
+        <v>0</v>
+      </c>
+      <c r="H38" s="32">
+        <v>0</v>
+      </c>
+      <c r="I38" s="32">
+        <v>0</v>
+      </c>
+      <c r="J38" s="32">
+        <v>45</v>
+      </c>
+      <c r="K38" s="32">
+        <v>50</v>
+      </c>
+      <c r="L38" s="32">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="32">
+        <v>13</v>
+      </c>
+      <c r="C39" s="32">
+        <v>0</v>
+      </c>
+      <c r="D39" s="32">
+        <v>0</v>
+      </c>
+      <c r="E39" s="32">
+        <v>0</v>
+      </c>
+      <c r="F39" s="32">
+        <v>1</v>
+      </c>
+      <c r="G39" s="32">
+        <v>0</v>
+      </c>
+      <c r="H39" s="32">
+        <v>0</v>
+      </c>
+      <c r="I39" s="32">
+        <v>0</v>
+      </c>
+      <c r="J39" s="32">
+        <v>42</v>
+      </c>
+      <c r="K39" s="32">
+        <v>56</v>
+      </c>
+      <c r="L39" s="32">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="B40" s="32">
+        <v>18</v>
+      </c>
+      <c r="C40" s="32">
+        <v>0</v>
+      </c>
+      <c r="D40" s="32">
+        <v>0</v>
+      </c>
+      <c r="E40" s="32">
+        <v>0</v>
+      </c>
+      <c r="F40" s="32">
+        <v>1</v>
+      </c>
+      <c r="G40" s="32">
+        <v>0</v>
+      </c>
+      <c r="H40" s="32">
+        <v>0</v>
+      </c>
+      <c r="I40" s="32">
+        <v>0</v>
+      </c>
+      <c r="J40" s="32">
+        <v>33</v>
+      </c>
+      <c r="K40" s="32">
+        <v>52</v>
+      </c>
+      <c r="L40" s="32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="B41" s="32">
+        <v>6</v>
+      </c>
+      <c r="C41" s="32">
+        <v>0</v>
+      </c>
+      <c r="D41" s="32">
+        <v>0</v>
+      </c>
+      <c r="E41" s="32">
+        <v>0</v>
+      </c>
+      <c r="F41" s="32">
+        <v>1</v>
+      </c>
+      <c r="G41" s="32">
+        <v>0</v>
+      </c>
+      <c r="H41" s="32">
+        <v>0</v>
+      </c>
+      <c r="I41" s="32">
+        <v>0</v>
+      </c>
+      <c r="J41" s="32">
+        <v>39</v>
+      </c>
+      <c r="K41" s="32">
+        <v>46</v>
+      </c>
+      <c r="L41" s="32">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="B42" s="32">
+        <v>2</v>
+      </c>
+      <c r="C42" s="32">
+        <v>0</v>
+      </c>
+      <c r="D42" s="32">
+        <v>0</v>
+      </c>
+      <c r="E42" s="32">
+        <v>0</v>
+      </c>
+      <c r="F42" s="32">
+        <v>1</v>
+      </c>
+      <c r="G42" s="32">
+        <v>0</v>
+      </c>
+      <c r="H42" s="32">
+        <v>0</v>
+      </c>
+      <c r="I42" s="32">
+        <v>0</v>
+      </c>
+      <c r="J42" s="32">
+        <v>21</v>
+      </c>
+      <c r="K42" s="32">
+        <v>24</v>
+      </c>
+      <c r="L42" s="32">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B43" s="32">
+        <v>10</v>
+      </c>
+      <c r="C43" s="32">
+        <v>0</v>
+      </c>
+      <c r="D43" s="32">
+        <v>0</v>
+      </c>
+      <c r="E43" s="32">
+        <v>0</v>
+      </c>
+      <c r="F43" s="32">
+        <v>1</v>
+      </c>
+      <c r="G43" s="32">
+        <v>0</v>
+      </c>
+      <c r="H43" s="32">
+        <v>0</v>
+      </c>
+      <c r="I43" s="32">
+        <v>0</v>
+      </c>
+      <c r="J43" s="32">
+        <v>35</v>
+      </c>
+      <c r="K43" s="32">
+        <v>46</v>
+      </c>
+      <c r="L43" s="32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B44" s="35">
+        <f>SUM(B2:B43)</f>
+        <v>387</v>
+      </c>
+      <c r="C44" s="35">
+        <f t="shared" ref="C44:L44" si="0">SUM(C2:C43)</f>
+        <v>12</v>
+      </c>
+      <c r="D44" s="35">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E44" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F44" s="35">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="G44" s="35">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+      <c r="H44" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="35">
+        <f t="shared" si="0"/>
+        <v>1684</v>
+      </c>
+      <c r="K44" s="35">
+        <f t="shared" si="0"/>
+        <v>2123</v>
+      </c>
+      <c r="L44" s="35">
+        <f t="shared" si="0"/>
+        <v>2522</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E45" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45" s="36">
+        <f>G44</f>
+        <v>103</v>
+      </c>
+      <c r="J45">
+        <f>B44-C44</f>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E46" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="36">
+        <f>B44</f>
+        <v>387</v>
+      </c>
+      <c r="J46">
+        <f>D44-E44</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E47" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="36">
+        <v>21</v>
+      </c>
+      <c r="J47">
+        <f>F53</f>
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E48" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J49" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f>SUM(F45:F49)</f>
+        <v>515</v>
+      </c>
+      <c r="J50">
+        <f>SUM(J45:J49)</f>
+        <v>2522</v>
+      </c>
+    </row>
+    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51">
+        <f>K44-F50</f>
+        <v>1608</v>
+      </c>
+      <c r="J51" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F52" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J52">
+        <f>J50-L44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f>F51+F50</f>
+        <v>2123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:J31"/>
   <sheetViews>

</xml_diff>

<commit_message>
nmv 13 05 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 7.1 TO 7.5.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 7.1 TO 7.5.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEEF83B-1E79-4608-AF96-A1887BAA85F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556C7C82-2116-4FF4-A685-53C466AE9ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="7.1" sheetId="15" r:id="rId1"/>
     <sheet name="7.2" sheetId="16" r:id="rId2"/>
     <sheet name="7.3" sheetId="17" r:id="rId3"/>
-    <sheet name="total 7.1 to 7.5" sheetId="7" r:id="rId4"/>
+    <sheet name="7.4" sheetId="18" r:id="rId4"/>
+    <sheet name="total 7.1 to 7.5" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="253">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1830,6 +1831,168 @@
   </si>
   <si>
     <t>42</t>
+  </si>
+  <si>
+    <t>7.4.1.1 :</t>
+  </si>
+  <si>
+    <t>7.4.1.2 :</t>
+  </si>
+  <si>
+    <t>7.4.1.3 :</t>
+  </si>
+  <si>
+    <t>7.4.2.1 :</t>
+  </si>
+  <si>
+    <t>7.4.2.2 :</t>
+  </si>
+  <si>
+    <t>7.4.2.3 :</t>
+  </si>
+  <si>
+    <t>7.4.2.4 :</t>
+  </si>
+  <si>
+    <t>7.4.2.5 :</t>
+  </si>
+  <si>
+    <t>7.4.3.1 :</t>
+  </si>
+  <si>
+    <t>7.4.3.2 :</t>
+  </si>
+  <si>
+    <t>7.4.3.3 :</t>
+  </si>
+  <si>
+    <t>7.4.3.4 :</t>
+  </si>
+  <si>
+    <t>7.4.3.5 :</t>
+  </si>
+  <si>
+    <t>7.4.3.6 :</t>
+  </si>
+  <si>
+    <t>7.4.4.1 :</t>
+  </si>
+  <si>
+    <t>7.4.4.2 :</t>
+  </si>
+  <si>
+    <t>7.4.4.3 :</t>
+  </si>
+  <si>
+    <t>7.4.5.1 :</t>
+  </si>
+  <si>
+    <t>7.4.5.2 :</t>
+  </si>
+  <si>
+    <t>7.4.5.3 :</t>
+  </si>
+  <si>
+    <t>7.4.5.4 :</t>
+  </si>
+  <si>
+    <t>7.4.6.1 :</t>
+  </si>
+  <si>
+    <t>7.4.6.2 :</t>
+  </si>
+  <si>
+    <t>7.4.6.3 :</t>
+  </si>
+  <si>
+    <t>7.4.7.1 :</t>
+  </si>
+  <si>
+    <t>7.4.7.2 :</t>
+  </si>
+  <si>
+    <t>7.4.7.3 :</t>
+  </si>
+  <si>
+    <t>7.4.8.1 :</t>
+  </si>
+  <si>
+    <t>7.4.8.2 :</t>
+  </si>
+  <si>
+    <t>7.4.8.3 :</t>
+  </si>
+  <si>
+    <t>7.4.9.1 :</t>
+  </si>
+  <si>
+    <t>7.4.10.1 :</t>
+  </si>
+  <si>
+    <t>7.4.10.2 :</t>
+  </si>
+  <si>
+    <t>7.4.11.1 :</t>
+  </si>
+  <si>
+    <t>7.4.11.2 :</t>
+  </si>
+  <si>
+    <t>7.4.11.3 :</t>
+  </si>
+  <si>
+    <t>7.4.11.4 :</t>
+  </si>
+  <si>
+    <t>7.4.12.1 :</t>
+  </si>
+  <si>
+    <t>7.4.13.1 :</t>
+  </si>
+  <si>
+    <t>7.4.14.1 :</t>
+  </si>
+  <si>
+    <t>7.4.15.1 :</t>
+  </si>
+  <si>
+    <t>7.4.16.1 :</t>
+  </si>
+  <si>
+    <t>7.4.17.1 :</t>
+  </si>
+  <si>
+    <t>7.4.17.2 :</t>
+  </si>
+  <si>
+    <t>7.4.18.1 :</t>
+  </si>
+  <si>
+    <t>7.4.18.2 :</t>
+  </si>
+  <si>
+    <t>7.4.19.1 :</t>
+  </si>
+  <si>
+    <t>7.4.19.2 :</t>
+  </si>
+  <si>
+    <t>7.4.19.3 :</t>
+  </si>
+  <si>
+    <t>7.4.19.4 :</t>
+  </si>
+  <si>
+    <t>7.4.20.1 :</t>
+  </si>
+  <si>
+    <t>7.4.21.1 :</t>
+  </si>
+  <si>
+    <t>7.4.22.1 :</t>
+  </si>
+  <si>
+    <t>53</t>
   </si>
 </sst>
 </file>
@@ -2032,7 +2195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2133,6 +2296,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6705,9 +6871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7653A96A-DC13-412E-A625-399CF21DC8FF}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44:L44"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45:K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8504,6 +8670,2227 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6597909C-BC93-461F-AFAC-454F999D36C1}">
+  <dimension ref="A1:L64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="32">
+        <v>6</v>
+      </c>
+      <c r="C2" s="32">
+        <v>0</v>
+      </c>
+      <c r="D2" s="32">
+        <v>0</v>
+      </c>
+      <c r="E2" s="32">
+        <v>0</v>
+      </c>
+      <c r="F2" s="32">
+        <v>0</v>
+      </c>
+      <c r="G2" s="32">
+        <v>1</v>
+      </c>
+      <c r="H2" s="32">
+        <v>0</v>
+      </c>
+      <c r="I2" s="32">
+        <v>0</v>
+      </c>
+      <c r="J2" s="32">
+        <v>44</v>
+      </c>
+      <c r="K2" s="32">
+        <v>50</v>
+      </c>
+      <c r="L2" s="32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="32">
+        <v>12</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0</v>
+      </c>
+      <c r="D3" s="32">
+        <v>0</v>
+      </c>
+      <c r="E3" s="32">
+        <v>0</v>
+      </c>
+      <c r="F3" s="32">
+        <v>0</v>
+      </c>
+      <c r="G3" s="32">
+        <v>2</v>
+      </c>
+      <c r="H3" s="32">
+        <v>0</v>
+      </c>
+      <c r="I3" s="32">
+        <v>0</v>
+      </c>
+      <c r="J3" s="32">
+        <v>38</v>
+      </c>
+      <c r="K3" s="32">
+        <v>50</v>
+      </c>
+      <c r="L3" s="32">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="32">
+        <v>15</v>
+      </c>
+      <c r="C4" s="32">
+        <v>1</v>
+      </c>
+      <c r="D4" s="32">
+        <v>5</v>
+      </c>
+      <c r="E4" s="32">
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <v>1</v>
+      </c>
+      <c r="G4" s="32">
+        <v>3</v>
+      </c>
+      <c r="H4" s="32">
+        <v>0</v>
+      </c>
+      <c r="I4" s="32">
+        <v>0</v>
+      </c>
+      <c r="J4" s="32">
+        <v>25</v>
+      </c>
+      <c r="K4" s="32">
+        <v>45</v>
+      </c>
+      <c r="L4" s="32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="32">
+        <v>7</v>
+      </c>
+      <c r="C5" s="32">
+        <v>0</v>
+      </c>
+      <c r="D5" s="32">
+        <v>0</v>
+      </c>
+      <c r="E5" s="32">
+        <v>0</v>
+      </c>
+      <c r="F5" s="32">
+        <v>0</v>
+      </c>
+      <c r="G5" s="32">
+        <v>1</v>
+      </c>
+      <c r="H5" s="32">
+        <v>0</v>
+      </c>
+      <c r="I5" s="32">
+        <v>0</v>
+      </c>
+      <c r="J5" s="32">
+        <v>43</v>
+      </c>
+      <c r="K5" s="32">
+        <v>50</v>
+      </c>
+      <c r="L5" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" s="32">
+        <v>18</v>
+      </c>
+      <c r="C6" s="32">
+        <v>0</v>
+      </c>
+      <c r="D6" s="32">
+        <v>0</v>
+      </c>
+      <c r="E6" s="32">
+        <v>0</v>
+      </c>
+      <c r="F6" s="32">
+        <v>0</v>
+      </c>
+      <c r="G6" s="32">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32">
+        <v>0</v>
+      </c>
+      <c r="I6" s="32">
+        <v>0</v>
+      </c>
+      <c r="J6" s="32">
+        <v>32</v>
+      </c>
+      <c r="K6" s="32">
+        <v>50</v>
+      </c>
+      <c r="L6" s="32">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="32">
+        <v>8</v>
+      </c>
+      <c r="C7" s="32">
+        <v>0</v>
+      </c>
+      <c r="D7" s="32">
+        <v>0</v>
+      </c>
+      <c r="E7" s="32">
+        <v>0</v>
+      </c>
+      <c r="F7" s="32">
+        <v>0</v>
+      </c>
+      <c r="G7" s="32">
+        <v>1</v>
+      </c>
+      <c r="H7" s="32">
+        <v>0</v>
+      </c>
+      <c r="I7" s="32">
+        <v>0</v>
+      </c>
+      <c r="J7" s="32">
+        <v>42</v>
+      </c>
+      <c r="K7" s="32">
+        <v>50</v>
+      </c>
+      <c r="L7" s="32">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="32">
+        <v>6</v>
+      </c>
+      <c r="C8" s="32">
+        <v>0</v>
+      </c>
+      <c r="D8" s="32">
+        <v>4</v>
+      </c>
+      <c r="E8" s="32">
+        <v>0</v>
+      </c>
+      <c r="F8" s="32">
+        <v>0</v>
+      </c>
+      <c r="G8" s="32">
+        <v>2</v>
+      </c>
+      <c r="H8" s="32">
+        <v>0</v>
+      </c>
+      <c r="I8" s="32">
+        <v>0</v>
+      </c>
+      <c r="J8" s="32">
+        <v>40</v>
+      </c>
+      <c r="K8" s="32">
+        <v>50</v>
+      </c>
+      <c r="L8" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9" s="32">
+        <v>26</v>
+      </c>
+      <c r="C9" s="32">
+        <v>1</v>
+      </c>
+      <c r="D9" s="32">
+        <v>2</v>
+      </c>
+      <c r="E9" s="32">
+        <v>0</v>
+      </c>
+      <c r="F9" s="32">
+        <v>1</v>
+      </c>
+      <c r="G9" s="32">
+        <v>5</v>
+      </c>
+      <c r="H9" s="32">
+        <v>0</v>
+      </c>
+      <c r="I9" s="32">
+        <v>0</v>
+      </c>
+      <c r="J9" s="32">
+        <v>46</v>
+      </c>
+      <c r="K9" s="32">
+        <v>74</v>
+      </c>
+      <c r="L9" s="32">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="32">
+        <v>10</v>
+      </c>
+      <c r="C10" s="32">
+        <v>0</v>
+      </c>
+      <c r="D10" s="32">
+        <v>0</v>
+      </c>
+      <c r="E10" s="32">
+        <v>0</v>
+      </c>
+      <c r="F10" s="32">
+        <v>0</v>
+      </c>
+      <c r="G10" s="32">
+        <v>4</v>
+      </c>
+      <c r="H10" s="32">
+        <v>0</v>
+      </c>
+      <c r="I10" s="32">
+        <v>0</v>
+      </c>
+      <c r="J10" s="32">
+        <v>40</v>
+      </c>
+      <c r="K10" s="32">
+        <v>50</v>
+      </c>
+      <c r="L10" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="32">
+        <v>13</v>
+      </c>
+      <c r="C11" s="32">
+        <v>0</v>
+      </c>
+      <c r="D11" s="32">
+        <v>0</v>
+      </c>
+      <c r="E11" s="32">
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <v>0</v>
+      </c>
+      <c r="G11" s="32">
+        <v>1</v>
+      </c>
+      <c r="H11" s="32">
+        <v>0</v>
+      </c>
+      <c r="I11" s="32">
+        <v>0</v>
+      </c>
+      <c r="J11" s="32">
+        <v>37</v>
+      </c>
+      <c r="K11" s="32">
+        <v>50</v>
+      </c>
+      <c r="L11" s="32">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="32">
+        <v>16</v>
+      </c>
+      <c r="C12" s="32">
+        <v>0</v>
+      </c>
+      <c r="D12" s="32">
+        <v>3</v>
+      </c>
+      <c r="E12" s="32">
+        <v>0</v>
+      </c>
+      <c r="F12" s="32">
+        <v>0</v>
+      </c>
+      <c r="G12" s="32">
+        <v>5</v>
+      </c>
+      <c r="H12" s="32">
+        <v>0</v>
+      </c>
+      <c r="I12" s="32">
+        <v>0</v>
+      </c>
+      <c r="J12" s="32">
+        <v>31</v>
+      </c>
+      <c r="K12" s="32">
+        <v>50</v>
+      </c>
+      <c r="L12" s="32">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B13" s="32">
+        <v>18</v>
+      </c>
+      <c r="C13" s="32">
+        <v>0</v>
+      </c>
+      <c r="D13" s="32">
+        <v>3</v>
+      </c>
+      <c r="E13" s="32">
+        <v>0</v>
+      </c>
+      <c r="F13" s="32">
+        <v>0</v>
+      </c>
+      <c r="G13" s="32">
+        <v>3</v>
+      </c>
+      <c r="H13" s="32">
+        <v>0</v>
+      </c>
+      <c r="I13" s="32">
+        <v>0</v>
+      </c>
+      <c r="J13" s="32">
+        <v>29</v>
+      </c>
+      <c r="K13" s="32">
+        <v>50</v>
+      </c>
+      <c r="L13" s="32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="32">
+        <v>13</v>
+      </c>
+      <c r="C14" s="32">
+        <v>0</v>
+      </c>
+      <c r="D14" s="32">
+        <v>1</v>
+      </c>
+      <c r="E14" s="32">
+        <v>0</v>
+      </c>
+      <c r="F14" s="32">
+        <v>0</v>
+      </c>
+      <c r="G14" s="32">
+        <v>3</v>
+      </c>
+      <c r="H14" s="32">
+        <v>0</v>
+      </c>
+      <c r="I14" s="32">
+        <v>0</v>
+      </c>
+      <c r="J14" s="32">
+        <v>36</v>
+      </c>
+      <c r="K14" s="32">
+        <v>50</v>
+      </c>
+      <c r="L14" s="32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" s="32">
+        <v>14</v>
+      </c>
+      <c r="C15" s="32">
+        <v>1</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0</v>
+      </c>
+      <c r="E15" s="32">
+        <v>0</v>
+      </c>
+      <c r="F15" s="32">
+        <v>1</v>
+      </c>
+      <c r="G15" s="32">
+        <v>1</v>
+      </c>
+      <c r="H15" s="32">
+        <v>0</v>
+      </c>
+      <c r="I15" s="32">
+        <v>0</v>
+      </c>
+      <c r="J15" s="32">
+        <v>35</v>
+      </c>
+      <c r="K15" s="32">
+        <v>49</v>
+      </c>
+      <c r="L15" s="32">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="32">
+        <v>15</v>
+      </c>
+      <c r="C16" s="32">
+        <v>0</v>
+      </c>
+      <c r="D16" s="32">
+        <v>0</v>
+      </c>
+      <c r="E16" s="32">
+        <v>0</v>
+      </c>
+      <c r="F16" s="32">
+        <v>0</v>
+      </c>
+      <c r="G16" s="32">
+        <v>2</v>
+      </c>
+      <c r="H16" s="32">
+        <v>0</v>
+      </c>
+      <c r="I16" s="32">
+        <v>0</v>
+      </c>
+      <c r="J16" s="32">
+        <v>35</v>
+      </c>
+      <c r="K16" s="32">
+        <v>50</v>
+      </c>
+      <c r="L16" s="32">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="B17" s="32">
+        <v>12</v>
+      </c>
+      <c r="C17" s="32">
+        <v>0</v>
+      </c>
+      <c r="D17" s="32">
+        <v>0</v>
+      </c>
+      <c r="E17" s="32">
+        <v>0</v>
+      </c>
+      <c r="F17" s="32">
+        <v>0</v>
+      </c>
+      <c r="G17" s="32">
+        <v>0</v>
+      </c>
+      <c r="H17" s="32">
+        <v>0</v>
+      </c>
+      <c r="I17" s="32">
+        <v>0</v>
+      </c>
+      <c r="J17" s="32">
+        <v>38</v>
+      </c>
+      <c r="K17" s="32">
+        <v>50</v>
+      </c>
+      <c r="L17" s="32">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="B18" s="32">
+        <v>17</v>
+      </c>
+      <c r="C18" s="32">
+        <v>1</v>
+      </c>
+      <c r="D18" s="32">
+        <v>9</v>
+      </c>
+      <c r="E18" s="32">
+        <v>0</v>
+      </c>
+      <c r="F18" s="32">
+        <v>1</v>
+      </c>
+      <c r="G18" s="32">
+        <v>3</v>
+      </c>
+      <c r="H18" s="32">
+        <v>0</v>
+      </c>
+      <c r="I18" s="32">
+        <v>0</v>
+      </c>
+      <c r="J18" s="32">
+        <v>46</v>
+      </c>
+      <c r="K18" s="32">
+        <v>72</v>
+      </c>
+      <c r="L18" s="32">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" s="32">
+        <v>11</v>
+      </c>
+      <c r="C19" s="32">
+        <v>0</v>
+      </c>
+      <c r="D19" s="32">
+        <v>2</v>
+      </c>
+      <c r="E19" s="32">
+        <v>0</v>
+      </c>
+      <c r="F19" s="32">
+        <v>0</v>
+      </c>
+      <c r="G19" s="32">
+        <v>3</v>
+      </c>
+      <c r="H19" s="32">
+        <v>0</v>
+      </c>
+      <c r="I19" s="32">
+        <v>0</v>
+      </c>
+      <c r="J19" s="32">
+        <v>37</v>
+      </c>
+      <c r="K19" s="32">
+        <v>50</v>
+      </c>
+      <c r="L19" s="32">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B20" s="32">
+        <v>8</v>
+      </c>
+      <c r="C20" s="32">
+        <v>0</v>
+      </c>
+      <c r="D20" s="32">
+        <v>1</v>
+      </c>
+      <c r="E20" s="32">
+        <v>0</v>
+      </c>
+      <c r="F20" s="32">
+        <v>0</v>
+      </c>
+      <c r="G20" s="32">
+        <v>3</v>
+      </c>
+      <c r="H20" s="32">
+        <v>0</v>
+      </c>
+      <c r="I20" s="32">
+        <v>0</v>
+      </c>
+      <c r="J20" s="32">
+        <v>41</v>
+      </c>
+      <c r="K20" s="32">
+        <v>50</v>
+      </c>
+      <c r="L20" s="32">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" s="32">
+        <v>11</v>
+      </c>
+      <c r="C21" s="32">
+        <v>0</v>
+      </c>
+      <c r="D21" s="32">
+        <v>1</v>
+      </c>
+      <c r="E21" s="32">
+        <v>0</v>
+      </c>
+      <c r="F21" s="32">
+        <v>0</v>
+      </c>
+      <c r="G21" s="32">
+        <v>5</v>
+      </c>
+      <c r="H21" s="32">
+        <v>0</v>
+      </c>
+      <c r="I21" s="32">
+        <v>0</v>
+      </c>
+      <c r="J21" s="32">
+        <v>38</v>
+      </c>
+      <c r="K21" s="32">
+        <v>50</v>
+      </c>
+      <c r="L21" s="32">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="B22" s="32">
+        <v>19</v>
+      </c>
+      <c r="C22" s="32">
+        <v>1</v>
+      </c>
+      <c r="D22" s="32">
+        <v>1</v>
+      </c>
+      <c r="E22" s="32">
+        <v>0</v>
+      </c>
+      <c r="F22" s="32">
+        <v>1</v>
+      </c>
+      <c r="G22" s="32">
+        <v>1</v>
+      </c>
+      <c r="H22" s="32">
+        <v>0</v>
+      </c>
+      <c r="I22" s="32">
+        <v>0</v>
+      </c>
+      <c r="J22" s="32">
+        <v>47</v>
+      </c>
+      <c r="K22" s="32">
+        <v>67</v>
+      </c>
+      <c r="L22" s="32">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" s="32">
+        <v>10</v>
+      </c>
+      <c r="C23" s="32">
+        <v>0</v>
+      </c>
+      <c r="D23" s="32">
+        <v>0</v>
+      </c>
+      <c r="E23" s="32">
+        <v>0</v>
+      </c>
+      <c r="F23" s="32">
+        <v>0</v>
+      </c>
+      <c r="G23" s="32">
+        <v>4</v>
+      </c>
+      <c r="H23" s="32">
+        <v>0</v>
+      </c>
+      <c r="I23" s="32">
+        <v>0</v>
+      </c>
+      <c r="J23" s="32">
+        <v>40</v>
+      </c>
+      <c r="K23" s="32">
+        <v>50</v>
+      </c>
+      <c r="L23" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="B24" s="32">
+        <v>7</v>
+      </c>
+      <c r="C24" s="32">
+        <v>0</v>
+      </c>
+      <c r="D24" s="32">
+        <v>0</v>
+      </c>
+      <c r="E24" s="32">
+        <v>0</v>
+      </c>
+      <c r="F24" s="32">
+        <v>0</v>
+      </c>
+      <c r="G24" s="32">
+        <v>3</v>
+      </c>
+      <c r="H24" s="32">
+        <v>0</v>
+      </c>
+      <c r="I24" s="32">
+        <v>0</v>
+      </c>
+      <c r="J24" s="32">
+        <v>43</v>
+      </c>
+      <c r="K24" s="32">
+        <v>50</v>
+      </c>
+      <c r="L24" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="B25" s="32">
+        <v>9</v>
+      </c>
+      <c r="C25" s="32">
+        <v>1</v>
+      </c>
+      <c r="D25" s="32">
+        <v>0</v>
+      </c>
+      <c r="E25" s="32">
+        <v>0</v>
+      </c>
+      <c r="F25" s="32">
+        <v>1</v>
+      </c>
+      <c r="G25" s="32">
+        <v>2</v>
+      </c>
+      <c r="H25" s="32">
+        <v>0</v>
+      </c>
+      <c r="I25" s="32">
+        <v>0</v>
+      </c>
+      <c r="J25" s="32">
+        <v>27</v>
+      </c>
+      <c r="K25" s="32">
+        <v>36</v>
+      </c>
+      <c r="L25" s="32">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" s="32">
+        <v>10</v>
+      </c>
+      <c r="C26" s="32">
+        <v>0</v>
+      </c>
+      <c r="D26" s="32">
+        <v>0</v>
+      </c>
+      <c r="E26" s="32">
+        <v>0</v>
+      </c>
+      <c r="F26" s="32">
+        <v>0</v>
+      </c>
+      <c r="G26" s="32">
+        <v>5</v>
+      </c>
+      <c r="H26" s="32">
+        <v>0</v>
+      </c>
+      <c r="I26" s="32">
+        <v>0</v>
+      </c>
+      <c r="J26" s="32">
+        <v>40</v>
+      </c>
+      <c r="K26" s="32">
+        <v>50</v>
+      </c>
+      <c r="L26" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="B27" s="32">
+        <v>11</v>
+      </c>
+      <c r="C27" s="32">
+        <v>0</v>
+      </c>
+      <c r="D27" s="32">
+        <v>2</v>
+      </c>
+      <c r="E27" s="32">
+        <v>0</v>
+      </c>
+      <c r="F27" s="32">
+        <v>0</v>
+      </c>
+      <c r="G27" s="32">
+        <v>3</v>
+      </c>
+      <c r="H27" s="32">
+        <v>0</v>
+      </c>
+      <c r="I27" s="32">
+        <v>0</v>
+      </c>
+      <c r="J27" s="32">
+        <v>37</v>
+      </c>
+      <c r="K27" s="32">
+        <v>50</v>
+      </c>
+      <c r="L27" s="32">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B28" s="32">
+        <v>17</v>
+      </c>
+      <c r="C28" s="32">
+        <v>1</v>
+      </c>
+      <c r="D28" s="32">
+        <v>0</v>
+      </c>
+      <c r="E28" s="32">
+        <v>0</v>
+      </c>
+      <c r="F28" s="32">
+        <v>1</v>
+      </c>
+      <c r="G28" s="32">
+        <v>3</v>
+      </c>
+      <c r="H28" s="32">
+        <v>0</v>
+      </c>
+      <c r="I28" s="32">
+        <v>0</v>
+      </c>
+      <c r="J28" s="32">
+        <v>55</v>
+      </c>
+      <c r="K28" s="32">
+        <v>72</v>
+      </c>
+      <c r="L28" s="32">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B29" s="32">
+        <v>15</v>
+      </c>
+      <c r="C29" s="32">
+        <v>0</v>
+      </c>
+      <c r="D29" s="32">
+        <v>2</v>
+      </c>
+      <c r="E29" s="32">
+        <v>0</v>
+      </c>
+      <c r="F29" s="32">
+        <v>0</v>
+      </c>
+      <c r="G29" s="32">
+        <v>2</v>
+      </c>
+      <c r="H29" s="32">
+        <v>0</v>
+      </c>
+      <c r="I29" s="32">
+        <v>0</v>
+      </c>
+      <c r="J29" s="32">
+        <v>33</v>
+      </c>
+      <c r="K29" s="32">
+        <v>50</v>
+      </c>
+      <c r="L29" s="32">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="B30" s="32">
+        <v>18</v>
+      </c>
+      <c r="C30" s="32">
+        <v>0</v>
+      </c>
+      <c r="D30" s="32">
+        <v>0</v>
+      </c>
+      <c r="E30" s="32">
+        <v>0</v>
+      </c>
+      <c r="F30" s="32">
+        <v>0</v>
+      </c>
+      <c r="G30" s="32">
+        <v>1</v>
+      </c>
+      <c r="H30" s="32">
+        <v>0</v>
+      </c>
+      <c r="I30" s="32">
+        <v>0</v>
+      </c>
+      <c r="J30" s="32">
+        <v>32</v>
+      </c>
+      <c r="K30" s="32">
+        <v>50</v>
+      </c>
+      <c r="L30" s="32">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="B31" s="32">
+        <v>4</v>
+      </c>
+      <c r="C31" s="32">
+        <v>0</v>
+      </c>
+      <c r="D31" s="32">
+        <v>0</v>
+      </c>
+      <c r="E31" s="32">
+        <v>0</v>
+      </c>
+      <c r="F31" s="32">
+        <v>1</v>
+      </c>
+      <c r="G31" s="32">
+        <v>9</v>
+      </c>
+      <c r="H31" s="32">
+        <v>0</v>
+      </c>
+      <c r="I31" s="32">
+        <v>0</v>
+      </c>
+      <c r="J31" s="32">
+        <v>29</v>
+      </c>
+      <c r="K31" s="32">
+        <v>34</v>
+      </c>
+      <c r="L31" s="32">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B32" s="32">
+        <v>6</v>
+      </c>
+      <c r="C32" s="32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="32">
+        <v>4</v>
+      </c>
+      <c r="H32" s="32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="32">
+        <v>0</v>
+      </c>
+      <c r="J32" s="32">
+        <v>42</v>
+      </c>
+      <c r="K32" s="32">
+        <v>50</v>
+      </c>
+      <c r="L32" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="B33" s="32">
+        <v>12</v>
+      </c>
+      <c r="C33" s="32">
+        <v>0</v>
+      </c>
+      <c r="D33" s="32">
+        <v>0</v>
+      </c>
+      <c r="E33" s="32">
+        <v>0</v>
+      </c>
+      <c r="F33" s="32">
+        <v>0</v>
+      </c>
+      <c r="G33" s="32">
+        <v>4</v>
+      </c>
+      <c r="H33" s="32">
+        <v>0</v>
+      </c>
+      <c r="I33" s="32">
+        <v>0</v>
+      </c>
+      <c r="J33" s="32">
+        <v>38</v>
+      </c>
+      <c r="K33" s="32">
+        <v>50</v>
+      </c>
+      <c r="L33" s="32">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B34" s="32">
+        <v>12</v>
+      </c>
+      <c r="C34" s="32">
+        <v>0</v>
+      </c>
+      <c r="D34" s="32">
+        <v>2</v>
+      </c>
+      <c r="E34" s="32">
+        <v>0</v>
+      </c>
+      <c r="F34" s="32">
+        <v>1</v>
+      </c>
+      <c r="G34" s="32">
+        <v>3</v>
+      </c>
+      <c r="H34" s="32">
+        <v>0</v>
+      </c>
+      <c r="I34" s="32">
+        <v>0</v>
+      </c>
+      <c r="J34" s="32">
+        <v>34</v>
+      </c>
+      <c r="K34" s="32">
+        <v>49</v>
+      </c>
+      <c r="L34" s="32">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" s="32">
+        <v>7</v>
+      </c>
+      <c r="C35" s="32">
+        <v>0</v>
+      </c>
+      <c r="D35" s="32">
+        <v>0</v>
+      </c>
+      <c r="E35" s="32">
+        <v>0</v>
+      </c>
+      <c r="F35" s="32">
+        <v>0</v>
+      </c>
+      <c r="G35" s="32">
+        <v>6</v>
+      </c>
+      <c r="H35" s="32">
+        <v>0</v>
+      </c>
+      <c r="I35" s="32">
+        <v>0</v>
+      </c>
+      <c r="J35" s="32">
+        <v>43</v>
+      </c>
+      <c r="K35" s="32">
+        <v>50</v>
+      </c>
+      <c r="L35" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="B36" s="32">
+        <v>7</v>
+      </c>
+      <c r="C36" s="32">
+        <v>0</v>
+      </c>
+      <c r="D36" s="32">
+        <v>3</v>
+      </c>
+      <c r="E36" s="32">
+        <v>0</v>
+      </c>
+      <c r="F36" s="32">
+        <v>0</v>
+      </c>
+      <c r="G36" s="32">
+        <v>5</v>
+      </c>
+      <c r="H36" s="32">
+        <v>0</v>
+      </c>
+      <c r="I36" s="32">
+        <v>0</v>
+      </c>
+      <c r="J36" s="32">
+        <v>40</v>
+      </c>
+      <c r="K36" s="32">
+        <v>50</v>
+      </c>
+      <c r="L36" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B37" s="32">
+        <v>8</v>
+      </c>
+      <c r="C37" s="32">
+        <v>0</v>
+      </c>
+      <c r="D37" s="32">
+        <v>2</v>
+      </c>
+      <c r="E37" s="32">
+        <v>0</v>
+      </c>
+      <c r="F37" s="32">
+        <v>0</v>
+      </c>
+      <c r="G37" s="32">
+        <v>3</v>
+      </c>
+      <c r="H37" s="32">
+        <v>0</v>
+      </c>
+      <c r="I37" s="32">
+        <v>0</v>
+      </c>
+      <c r="J37" s="32">
+        <v>40</v>
+      </c>
+      <c r="K37" s="32">
+        <v>50</v>
+      </c>
+      <c r="L37" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B38" s="32">
+        <v>19</v>
+      </c>
+      <c r="C38" s="32">
+        <v>0</v>
+      </c>
+      <c r="D38" s="32">
+        <v>0</v>
+      </c>
+      <c r="E38" s="32">
+        <v>0</v>
+      </c>
+      <c r="F38" s="32">
+        <v>1</v>
+      </c>
+      <c r="G38" s="32">
+        <v>5</v>
+      </c>
+      <c r="H38" s="32">
+        <v>0</v>
+      </c>
+      <c r="I38" s="32">
+        <v>0</v>
+      </c>
+      <c r="J38" s="32">
+        <v>38</v>
+      </c>
+      <c r="K38" s="32">
+        <v>58</v>
+      </c>
+      <c r="L38" s="32">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="B39" s="32">
+        <v>5</v>
+      </c>
+      <c r="C39" s="32">
+        <v>0</v>
+      </c>
+      <c r="D39" s="32">
+        <v>1</v>
+      </c>
+      <c r="E39" s="32">
+        <v>0</v>
+      </c>
+      <c r="F39" s="32">
+        <v>1</v>
+      </c>
+      <c r="G39" s="32">
+        <v>0</v>
+      </c>
+      <c r="H39" s="32">
+        <v>0</v>
+      </c>
+      <c r="I39" s="32">
+        <v>0</v>
+      </c>
+      <c r="J39" s="32">
+        <v>29</v>
+      </c>
+      <c r="K39" s="32">
+        <v>36</v>
+      </c>
+      <c r="L39" s="32">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="B40" s="32">
+        <v>2</v>
+      </c>
+      <c r="C40" s="32">
+        <v>0</v>
+      </c>
+      <c r="D40" s="32">
+        <v>0</v>
+      </c>
+      <c r="E40" s="32">
+        <v>0</v>
+      </c>
+      <c r="F40" s="32">
+        <v>1</v>
+      </c>
+      <c r="G40" s="32">
+        <v>0</v>
+      </c>
+      <c r="H40" s="32">
+        <v>0</v>
+      </c>
+      <c r="I40" s="32">
+        <v>0</v>
+      </c>
+      <c r="J40" s="32">
+        <v>37</v>
+      </c>
+      <c r="K40" s="32">
+        <v>40</v>
+      </c>
+      <c r="L40" s="32">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="B41" s="32">
+        <v>6</v>
+      </c>
+      <c r="C41" s="32">
+        <v>0</v>
+      </c>
+      <c r="D41" s="32">
+        <v>0</v>
+      </c>
+      <c r="E41" s="32">
+        <v>0</v>
+      </c>
+      <c r="F41" s="32">
+        <v>1</v>
+      </c>
+      <c r="G41" s="32">
+        <v>0</v>
+      </c>
+      <c r="H41" s="32">
+        <v>0</v>
+      </c>
+      <c r="I41" s="32">
+        <v>0</v>
+      </c>
+      <c r="J41" s="32">
+        <v>22</v>
+      </c>
+      <c r="K41" s="32">
+        <v>29</v>
+      </c>
+      <c r="L41" s="32">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="B42" s="32">
+        <v>3</v>
+      </c>
+      <c r="C42" s="32">
+        <v>0</v>
+      </c>
+      <c r="D42" s="32">
+        <v>0</v>
+      </c>
+      <c r="E42" s="32">
+        <v>0</v>
+      </c>
+      <c r="F42" s="32">
+        <v>6</v>
+      </c>
+      <c r="G42" s="32">
+        <v>4</v>
+      </c>
+      <c r="H42" s="32">
+        <v>0</v>
+      </c>
+      <c r="I42" s="32">
+        <v>0</v>
+      </c>
+      <c r="J42" s="32">
+        <v>43</v>
+      </c>
+      <c r="K42" s="32">
+        <v>52</v>
+      </c>
+      <c r="L42" s="32">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="B43" s="32">
+        <v>8</v>
+      </c>
+      <c r="C43" s="32">
+        <v>0</v>
+      </c>
+      <c r="D43" s="32">
+        <v>0</v>
+      </c>
+      <c r="E43" s="32">
+        <v>0</v>
+      </c>
+      <c r="F43" s="32">
+        <v>1</v>
+      </c>
+      <c r="G43" s="32">
+        <v>0</v>
+      </c>
+      <c r="H43" s="32">
+        <v>0</v>
+      </c>
+      <c r="I43" s="32">
+        <v>0</v>
+      </c>
+      <c r="J43" s="32">
+        <v>20</v>
+      </c>
+      <c r="K43" s="32">
+        <v>29</v>
+      </c>
+      <c r="L43" s="32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="B44" s="32">
+        <v>8</v>
+      </c>
+      <c r="C44" s="32">
+        <v>0</v>
+      </c>
+      <c r="D44" s="32">
+        <v>0</v>
+      </c>
+      <c r="E44" s="32">
+        <v>0</v>
+      </c>
+      <c r="F44" s="32">
+        <v>5</v>
+      </c>
+      <c r="G44" s="32">
+        <v>2</v>
+      </c>
+      <c r="H44" s="32">
+        <v>0</v>
+      </c>
+      <c r="I44" s="32">
+        <v>0</v>
+      </c>
+      <c r="J44" s="32">
+        <v>37</v>
+      </c>
+      <c r="K44" s="32">
+        <v>50</v>
+      </c>
+      <c r="L44" s="32">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="B45" s="32">
+        <v>8</v>
+      </c>
+      <c r="C45" s="32">
+        <v>2</v>
+      </c>
+      <c r="D45" s="32">
+        <v>0</v>
+      </c>
+      <c r="E45" s="32">
+        <v>0</v>
+      </c>
+      <c r="F45" s="32">
+        <v>4</v>
+      </c>
+      <c r="G45" s="32">
+        <v>4</v>
+      </c>
+      <c r="H45" s="32">
+        <v>0</v>
+      </c>
+      <c r="I45" s="32">
+        <v>0</v>
+      </c>
+      <c r="J45" s="32">
+        <v>28</v>
+      </c>
+      <c r="K45" s="32">
+        <v>38</v>
+      </c>
+      <c r="L45" s="32">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" s="32">
+        <v>3</v>
+      </c>
+      <c r="C46" s="32">
+        <v>0</v>
+      </c>
+      <c r="D46" s="32">
+        <v>0</v>
+      </c>
+      <c r="E46" s="32">
+        <v>0</v>
+      </c>
+      <c r="F46" s="32">
+        <v>6</v>
+      </c>
+      <c r="G46" s="32">
+        <v>0</v>
+      </c>
+      <c r="H46" s="32">
+        <v>0</v>
+      </c>
+      <c r="I46" s="32">
+        <v>0</v>
+      </c>
+      <c r="J46" s="32">
+        <v>41</v>
+      </c>
+      <c r="K46" s="32">
+        <v>50</v>
+      </c>
+      <c r="L46" s="32">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="B47" s="32">
+        <v>3</v>
+      </c>
+      <c r="C47" s="32">
+        <v>2</v>
+      </c>
+      <c r="D47" s="32">
+        <v>0</v>
+      </c>
+      <c r="E47" s="32">
+        <v>0</v>
+      </c>
+      <c r="F47" s="32">
+        <v>6</v>
+      </c>
+      <c r="G47" s="32">
+        <v>0</v>
+      </c>
+      <c r="H47" s="32">
+        <v>0</v>
+      </c>
+      <c r="I47" s="32">
+        <v>0</v>
+      </c>
+      <c r="J47" s="32">
+        <v>39</v>
+      </c>
+      <c r="K47" s="32">
+        <v>46</v>
+      </c>
+      <c r="L47" s="32">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B48" s="32">
+        <v>8</v>
+      </c>
+      <c r="C48" s="32">
+        <v>1</v>
+      </c>
+      <c r="D48" s="32">
+        <v>0</v>
+      </c>
+      <c r="E48" s="32">
+        <v>0</v>
+      </c>
+      <c r="F48" s="32">
+        <v>6</v>
+      </c>
+      <c r="G48" s="32">
+        <v>8</v>
+      </c>
+      <c r="H48" s="32">
+        <v>0</v>
+      </c>
+      <c r="I48" s="32">
+        <v>0</v>
+      </c>
+      <c r="J48" s="32">
+        <v>37</v>
+      </c>
+      <c r="K48" s="32">
+        <v>50</v>
+      </c>
+      <c r="L48" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="B49" s="32">
+        <v>3</v>
+      </c>
+      <c r="C49" s="32">
+        <v>2</v>
+      </c>
+      <c r="D49" s="32">
+        <v>0</v>
+      </c>
+      <c r="E49" s="32">
+        <v>0</v>
+      </c>
+      <c r="F49" s="32">
+        <v>9</v>
+      </c>
+      <c r="G49" s="32">
+        <v>1</v>
+      </c>
+      <c r="H49" s="32">
+        <v>0</v>
+      </c>
+      <c r="I49" s="32">
+        <v>0</v>
+      </c>
+      <c r="J49" s="32">
+        <v>40</v>
+      </c>
+      <c r="K49" s="32">
+        <v>50</v>
+      </c>
+      <c r="L49" s="32">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="B50" s="32">
+        <v>3</v>
+      </c>
+      <c r="C50" s="32">
+        <v>0</v>
+      </c>
+      <c r="D50" s="32">
+        <v>0</v>
+      </c>
+      <c r="E50" s="32">
+        <v>0</v>
+      </c>
+      <c r="F50" s="32">
+        <v>9</v>
+      </c>
+      <c r="G50" s="32">
+        <v>1</v>
+      </c>
+      <c r="H50" s="32">
+        <v>0</v>
+      </c>
+      <c r="I50" s="32">
+        <v>0</v>
+      </c>
+      <c r="J50" s="32">
+        <v>38</v>
+      </c>
+      <c r="K50" s="32">
+        <v>50</v>
+      </c>
+      <c r="L50" s="32">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B51" s="32">
+        <v>3</v>
+      </c>
+      <c r="C51" s="32">
+        <v>0</v>
+      </c>
+      <c r="D51" s="32">
+        <v>0</v>
+      </c>
+      <c r="E51" s="32">
+        <v>0</v>
+      </c>
+      <c r="F51" s="32">
+        <v>9</v>
+      </c>
+      <c r="G51" s="32">
+        <v>2</v>
+      </c>
+      <c r="H51" s="32">
+        <v>0</v>
+      </c>
+      <c r="I51" s="32">
+        <v>0</v>
+      </c>
+      <c r="J51" s="32">
+        <v>42</v>
+      </c>
+      <c r="K51" s="32">
+        <v>54</v>
+      </c>
+      <c r="L51" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="B52" s="32">
+        <v>4</v>
+      </c>
+      <c r="C52" s="32">
+        <v>2</v>
+      </c>
+      <c r="D52" s="32">
+        <v>2</v>
+      </c>
+      <c r="E52" s="32">
+        <v>0</v>
+      </c>
+      <c r="F52" s="32">
+        <v>10</v>
+      </c>
+      <c r="G52" s="32">
+        <v>3</v>
+      </c>
+      <c r="H52" s="32">
+        <v>0</v>
+      </c>
+      <c r="I52" s="32">
+        <v>0</v>
+      </c>
+      <c r="J52" s="32">
+        <v>61</v>
+      </c>
+      <c r="K52" s="32">
+        <v>75</v>
+      </c>
+      <c r="L52" s="32">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="B53" s="32">
+        <v>9</v>
+      </c>
+      <c r="C53" s="32">
+        <v>0</v>
+      </c>
+      <c r="D53" s="32">
+        <v>0</v>
+      </c>
+      <c r="E53" s="32">
+        <v>0</v>
+      </c>
+      <c r="F53" s="32">
+        <v>1</v>
+      </c>
+      <c r="G53" s="32">
+        <v>0</v>
+      </c>
+      <c r="H53" s="32">
+        <v>0</v>
+      </c>
+      <c r="I53" s="32">
+        <v>0</v>
+      </c>
+      <c r="J53" s="32">
+        <v>18</v>
+      </c>
+      <c r="K53" s="32">
+        <v>28</v>
+      </c>
+      <c r="L53" s="32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="B54" s="32">
+        <v>10</v>
+      </c>
+      <c r="C54" s="32">
+        <v>0</v>
+      </c>
+      <c r="D54" s="32">
+        <v>0</v>
+      </c>
+      <c r="E54" s="32">
+        <v>0</v>
+      </c>
+      <c r="F54" s="32">
+        <v>1</v>
+      </c>
+      <c r="G54" s="32">
+        <v>0</v>
+      </c>
+      <c r="H54" s="32">
+        <v>0</v>
+      </c>
+      <c r="I54" s="32">
+        <v>0</v>
+      </c>
+      <c r="J54" s="32">
+        <v>27</v>
+      </c>
+      <c r="K54" s="32">
+        <v>38</v>
+      </c>
+      <c r="L54" s="32">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="B55" s="35">
+        <f>SUM(B2:B54)</f>
+        <v>533</v>
+      </c>
+      <c r="C55" s="35">
+        <f t="shared" ref="C55:L55" si="0">SUM(C2:C54)</f>
+        <v>16</v>
+      </c>
+      <c r="D55" s="35">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="E55" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="35">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="G55" s="35">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="H55" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I55" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="35">
+        <f t="shared" si="0"/>
+        <v>1970</v>
+      </c>
+      <c r="K55" s="35">
+        <f t="shared" si="0"/>
+        <v>2621</v>
+      </c>
+      <c r="L55" s="35">
+        <f t="shared" si="0"/>
+        <v>3185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="39"/>
+      <c r="E56" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F56" s="36">
+        <f>G55</f>
+        <v>136</v>
+      </c>
+      <c r="J56">
+        <f>B55-C55</f>
+        <v>517</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E57" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="36">
+        <f>B55</f>
+        <v>533</v>
+      </c>
+      <c r="J57">
+        <f>D55-E55</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E58" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F58" s="36">
+        <v>41</v>
+      </c>
+      <c r="J58">
+        <f>F64</f>
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E59" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F59" s="36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F60" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J60" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <f>SUM(F56:F60)</f>
+        <v>716</v>
+      </c>
+      <c r="J61">
+        <f>SUM(J56:J60)</f>
+        <v>3185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>45</v>
+      </c>
+      <c r="F62">
+        <f>K55-F61</f>
+        <v>1905</v>
+      </c>
+      <c r="J62" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F63" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J63">
+        <f>J61-L55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f>F62+F61</f>
+        <v>2621</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:J31"/>
   <sheetViews>

</xml_diff>